<commit_message>
fix preoblem with pine and elm data
</commit_message>
<xml_diff>
--- a/data/trees-cost-benefit.xlsx
+++ b/data/trees-cost-benefit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunaynaagarwal/Documents/GitHub/capstone project/urbanforest_CBA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8B79CF-4294-E345-A996-1588281A320F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7416C0-E355-5E4D-990D-B3E0FFCBEBB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="460" windowWidth="25040" windowHeight="14100" xr2:uid="{2A928EC9-B78E-A343-8FB2-6539B0E6B4D7}"/>
   </bookViews>
@@ -59,13 +59,7 @@
     <t>blue palo verde</t>
   </si>
   <si>
-    <t xml:space="preserve">aleppo pine </t>
-  </si>
-  <si>
     <t>palo brea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chinese elm </t>
   </si>
   <si>
     <t>ben_property_value</t>
@@ -102,6 +96,12 @@
   </si>
   <si>
     <t>convenient</t>
+  </si>
+  <si>
+    <t>chinese elm</t>
+  </si>
+  <si>
+    <t>aleppo pine</t>
   </si>
 </sst>
 </file>
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C43A03F-FC37-6C4A-BA3B-39FF00DA712F}">
   <dimension ref="A1:S311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
-      <selection activeCell="L311" sqref="L311"/>
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="A251" sqref="A251:A311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,34 +497,34 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -568,7 +568,7 @@
         <v>0.37</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N2" s="3">
         <v>8.5299999999999994</v>
@@ -618,7 +618,7 @@
         <v>0.47</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N3" s="3">
         <v>10.940000000000001</v>
@@ -668,7 +668,7 @@
         <v>0.63</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N4" s="3">
         <v>13.060000000000002</v>
@@ -718,7 +718,7 @@
         <v>1.03</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N5" s="3">
         <v>14.22</v>
@@ -768,7 +768,7 @@
         <v>1.42</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N6" s="3">
         <v>15.679999999999998</v>
@@ -818,7 +818,7 @@
         <v>1.81</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N7" s="3">
         <v>16.970000000000002</v>
@@ -868,7 +868,7 @@
         <v>2.21</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N8" s="3">
         <v>18.279999999999998</v>
@@ -918,7 +918,7 @@
         <v>2.6</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N9" s="3">
         <v>19.55</v>
@@ -968,7 +968,7 @@
         <v>2.99</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N10" s="3">
         <v>20.86</v>
@@ -1018,7 +1018,7 @@
         <v>3.39</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N11" s="3">
         <v>22.15</v>
@@ -1068,7 +1068,7 @@
         <v>3.78</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N12" s="3">
         <v>23.43</v>
@@ -1118,7 +1118,7 @@
         <v>4.18</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N13" s="3">
         <v>24.73</v>
@@ -1168,7 +1168,7 @@
         <v>4.57</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N14" s="3">
         <v>26.020000000000003</v>
@@ -1218,7 +1218,7 @@
         <v>5.04</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N15" s="3">
         <v>27.43</v>
@@ -1268,7 +1268,7 @@
         <v>5.6</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N16" s="3">
         <v>28.97</v>
@@ -1318,7 +1318,7 @@
         <v>6.15</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N17" s="3">
         <v>30.490000000000002</v>
@@ -1368,7 +1368,7 @@
         <v>6.71</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N18" s="3">
         <v>32.03</v>
@@ -1418,7 +1418,7 @@
         <v>7.26</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N19" s="3">
         <v>33.549999999999997</v>
@@ -1468,7 +1468,7 @@
         <v>7.8</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N20" s="3">
         <v>35.03</v>
@@ -1518,7 +1518,7 @@
         <v>8.31</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N21" s="3">
         <v>36.449999999999996</v>
@@ -1568,7 +1568,7 @@
         <v>8.81</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N22" s="3">
         <v>37.82</v>
@@ -1618,7 +1618,7 @@
         <v>9.2899999999999991</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N23" s="3">
         <v>39.14</v>
@@ -1668,7 +1668,7 @@
         <v>9.7200000000000006</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N24" s="3">
         <v>40.32</v>
@@ -1718,7 +1718,7 @@
         <v>10.14</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N25" s="3">
         <v>41.480000000000004</v>
@@ -1768,7 +1768,7 @@
         <v>10.53</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N26" s="3">
         <v>42.570000000000007</v>
@@ -1818,7 +1818,7 @@
         <v>10.93</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N27" s="3">
         <v>43.67</v>
@@ -1868,7 +1868,7 @@
         <v>11.31</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N28" s="3">
         <v>44.71</v>
@@ -1918,7 +1918,7 @@
         <v>11.66</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N29" s="3">
         <v>45.69</v>
@@ -1968,7 +1968,7 @@
         <v>12</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N30" s="3">
         <v>46.620000000000005</v>
@@ -2018,7 +2018,7 @@
         <v>12.34</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N31" s="3">
         <v>47.56</v>
@@ -2068,7 +2068,7 @@
         <v>12.68</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N32" s="3">
         <v>48.49</v>
@@ -2118,7 +2118,7 @@
         <v>0.37</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N33" s="3">
         <v>8.5299999999999994</v>
@@ -2168,7 +2168,7 @@
         <v>0.47</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N34" s="3">
         <v>10.940000000000001</v>
@@ -2218,7 +2218,7 @@
         <v>0.63</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N35" s="3">
         <v>13.060000000000002</v>
@@ -2268,7 +2268,7 @@
         <v>1.03</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N36" s="3">
         <v>14.22</v>
@@ -2318,7 +2318,7 @@
         <v>1.42</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N37" s="3">
         <v>15.679999999999998</v>
@@ -2368,7 +2368,7 @@
         <v>1.81</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N38" s="3">
         <v>16.970000000000002</v>
@@ -2418,7 +2418,7 @@
         <v>2.21</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N39" s="3">
         <v>18.279999999999998</v>
@@ -2468,7 +2468,7 @@
         <v>2.6</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N40" s="3">
         <v>19.55</v>
@@ -2518,7 +2518,7 @@
         <v>2.99</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N41" s="3">
         <v>20.86</v>
@@ -2568,7 +2568,7 @@
         <v>3.39</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N42" s="3">
         <v>22.15</v>
@@ -2618,7 +2618,7 @@
         <v>3.78</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N43" s="3">
         <v>23.43</v>
@@ -2668,7 +2668,7 @@
         <v>4.18</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N44" s="3">
         <v>24.73</v>
@@ -2718,7 +2718,7 @@
         <v>4.57</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N45" s="3">
         <v>26.020000000000003</v>
@@ -2768,7 +2768,7 @@
         <v>5.04</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N46" s="3">
         <v>27.43</v>
@@ -2818,7 +2818,7 @@
         <v>5.6</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N47" s="3">
         <v>28.97</v>
@@ -2868,7 +2868,7 @@
         <v>6.15</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N48" s="3">
         <v>30.490000000000002</v>
@@ -2918,7 +2918,7 @@
         <v>6.71</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N49" s="3">
         <v>32.03</v>
@@ -2968,7 +2968,7 @@
         <v>0.37</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N50" s="3">
         <v>8.5299999999999994</v>
@@ -3018,7 +3018,7 @@
         <v>0.47</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N51" s="3">
         <v>10.940000000000001</v>
@@ -3068,7 +3068,7 @@
         <v>0.63</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N52" s="3">
         <v>13.060000000000002</v>
@@ -3118,7 +3118,7 @@
         <v>1.03</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N53" s="3">
         <v>14.22</v>
@@ -3168,7 +3168,7 @@
         <v>1.42</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N54" s="3">
         <v>15.679999999999998</v>
@@ -3218,7 +3218,7 @@
         <v>1.81</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N55" s="3">
         <v>16.970000000000002</v>
@@ -3268,7 +3268,7 @@
         <v>2.21</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N56" s="3">
         <v>18.279999999999998</v>
@@ -3318,7 +3318,7 @@
         <v>2.6</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N57" s="3">
         <v>19.55</v>
@@ -3368,7 +3368,7 @@
         <v>2.99</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N58" s="3">
         <v>20.86</v>
@@ -3418,7 +3418,7 @@
         <v>3.39</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N59" s="3">
         <v>22.15</v>
@@ -3468,7 +3468,7 @@
         <v>3.78</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N60" s="3">
         <v>23.43</v>
@@ -3518,7 +3518,7 @@
         <v>4.18</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N61" s="3">
         <v>24.73</v>
@@ -3568,7 +3568,7 @@
         <v>4.57</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N62" s="3">
         <v>26.020000000000003</v>
@@ -3618,7 +3618,7 @@
         <v>5.04</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N63" s="3">
         <v>27.43</v>
@@ -3668,7 +3668,7 @@
         <v>0.37</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N64" s="3">
         <v>4.3599999999999994</v>
@@ -3718,7 +3718,7 @@
         <v>0.5</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N65" s="3">
         <v>5.93</v>
@@ -3768,7 +3768,7 @@
         <v>0.9</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N66" s="3">
         <v>7.620000000000001</v>
@@ -3818,7 +3818,7 @@
         <v>1.48</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N67" s="3">
         <v>9.3199999999999985</v>
@@ -3868,7 +3868,7 @@
         <v>2.06</v>
       </c>
       <c r="M68" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N68" s="3">
         <v>11.060000000000002</v>
@@ -3918,7 +3918,7 @@
         <v>2.64</v>
       </c>
       <c r="M69" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N69" s="3">
         <v>12.780000000000001</v>
@@ -3968,7 +3968,7 @@
         <v>3.21</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N70" s="3">
         <v>14.52</v>
@@ -4018,7 +4018,7 @@
         <v>3.79</v>
       </c>
       <c r="M71" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N71" s="3">
         <v>16.240000000000002</v>
@@ -4068,7 +4068,7 @@
         <v>4.37</v>
       </c>
       <c r="M72" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N72" s="3">
         <v>17.97</v>
@@ -4118,7 +4118,7 @@
         <v>4.95</v>
       </c>
       <c r="M73" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N73" s="3">
         <v>19.7</v>
@@ -4168,7 +4168,7 @@
         <v>5.55</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N74" s="3">
         <v>21.51</v>
@@ -4218,7 +4218,7 @@
         <v>6.29</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N75" s="3">
         <v>23.729999999999997</v>
@@ -4268,7 +4268,7 @@
         <v>6.97</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N76" s="3">
         <v>25.77</v>
@@ -4318,7 +4318,7 @@
         <v>7.59</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N77" s="3">
         <v>27.62</v>
@@ -4368,7 +4368,7 @@
         <v>8.16</v>
       </c>
       <c r="M78" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N78" s="3">
         <v>29.319999999999997</v>
@@ -4418,7 +4418,7 @@
         <v>8.82</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N79" s="3">
         <v>31.310000000000002</v>
@@ -4468,7 +4468,7 @@
         <v>9.34</v>
       </c>
       <c r="M80" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N80" s="3">
         <v>32.879999999999995</v>
@@ -4518,7 +4518,7 @@
         <v>9.7899999999999991</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N81" s="3">
         <v>34.119999999999997</v>
@@ -4568,7 +4568,7 @@
         <v>10.19</v>
       </c>
       <c r="M82" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N82" s="3">
         <v>35.44</v>
@@ -4618,7 +4618,7 @@
         <v>10.57</v>
       </c>
       <c r="M83" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N83" s="3">
         <v>36.570000000000007</v>
@@ -4668,7 +4668,7 @@
         <v>10.93</v>
       </c>
       <c r="M84" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N84" s="3">
         <v>37.650000000000006</v>
@@ -4718,7 +4718,7 @@
         <v>11.26</v>
       </c>
       <c r="M85" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N85" s="3">
         <v>38.639999999999993</v>
@@ -4768,7 +4768,7 @@
         <v>11.57</v>
       </c>
       <c r="M86" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N86" s="3">
         <v>39.57</v>
@@ -4818,7 +4818,7 @@
         <v>11.85</v>
       </c>
       <c r="M87" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N87" s="3">
         <v>40.410000000000004</v>
@@ -4868,7 +4868,7 @@
         <v>12.11</v>
       </c>
       <c r="M88" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N88" s="3">
         <v>41.18</v>
@@ -4918,7 +4918,7 @@
         <v>12.35</v>
       </c>
       <c r="M89" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N89" s="3">
         <v>41.9</v>
@@ -4968,7 +4968,7 @@
         <v>12.56</v>
       </c>
       <c r="M90" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N90" s="3">
         <v>42.54</v>
@@ -5018,7 +5018,7 @@
         <v>12.78</v>
       </c>
       <c r="M91" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N91" s="3">
         <v>43.18</v>
@@ -5068,7 +5068,7 @@
         <v>12.97</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N92" s="3">
         <v>43.75</v>
@@ -5118,7 +5118,7 @@
         <v>13.16</v>
       </c>
       <c r="M93" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N93" s="3">
         <v>44.319999999999993</v>
@@ -5168,7 +5168,7 @@
         <v>13.32</v>
       </c>
       <c r="M94" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N94" s="3">
         <v>44.81</v>
@@ -5218,7 +5218,7 @@
         <v>0.37</v>
       </c>
       <c r="M95" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N95" s="3">
         <v>4.3599999999999994</v>
@@ -5268,7 +5268,7 @@
         <v>0.5</v>
       </c>
       <c r="M96" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N96" s="3">
         <v>5.93</v>
@@ -5318,7 +5318,7 @@
         <v>0.9</v>
       </c>
       <c r="M97" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N97" s="3">
         <v>7.620000000000001</v>
@@ -5368,7 +5368,7 @@
         <v>1.48</v>
       </c>
       <c r="M98" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N98" s="3">
         <v>9.3199999999999985</v>
@@ -5418,7 +5418,7 @@
         <v>2.06</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N99" s="3">
         <v>11.060000000000002</v>
@@ -5468,7 +5468,7 @@
         <v>2.64</v>
       </c>
       <c r="M100" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N100" s="3">
         <v>12.780000000000001</v>
@@ -5518,7 +5518,7 @@
         <v>3.21</v>
       </c>
       <c r="M101" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N101" s="3">
         <v>14.52</v>
@@ -5568,7 +5568,7 @@
         <v>3.79</v>
       </c>
       <c r="M102" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N102" s="3">
         <v>16.240000000000002</v>
@@ -5618,7 +5618,7 @@
         <v>4.37</v>
       </c>
       <c r="M103" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N103" s="3">
         <v>17.97</v>
@@ -5668,7 +5668,7 @@
         <v>4.95</v>
       </c>
       <c r="M104" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N104" s="3">
         <v>19.7</v>
@@ -5718,7 +5718,7 @@
         <v>5.55</v>
       </c>
       <c r="M105" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N105" s="3">
         <v>21.51</v>
@@ -5768,7 +5768,7 @@
         <v>6.29</v>
       </c>
       <c r="M106" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N106" s="3">
         <v>23.729999999999997</v>
@@ -5818,7 +5818,7 @@
         <v>6.97</v>
       </c>
       <c r="M107" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N107" s="3">
         <v>25.77</v>
@@ -5868,7 +5868,7 @@
         <v>7.59</v>
       </c>
       <c r="M108" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N108" s="3">
         <v>27.62</v>
@@ -5918,7 +5918,7 @@
         <v>8.16</v>
       </c>
       <c r="M109" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N109" s="3">
         <v>29.319999999999997</v>
@@ -5968,7 +5968,7 @@
         <v>0.37</v>
       </c>
       <c r="M110" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N110" s="3">
         <v>4.3599999999999994</v>
@@ -6018,7 +6018,7 @@
         <v>0.5</v>
       </c>
       <c r="M111" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N111" s="3">
         <v>5.93</v>
@@ -6068,7 +6068,7 @@
         <v>0.9</v>
       </c>
       <c r="M112" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N112" s="3">
         <v>7.620000000000001</v>
@@ -6118,7 +6118,7 @@
         <v>1.48</v>
       </c>
       <c r="M113" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N113" s="3">
         <v>9.3199999999999985</v>
@@ -6168,7 +6168,7 @@
         <v>2.06</v>
       </c>
       <c r="M114" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N114" s="3">
         <v>11.060000000000002</v>
@@ -6218,7 +6218,7 @@
         <v>2.64</v>
       </c>
       <c r="M115" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N115" s="3">
         <v>12.780000000000001</v>
@@ -6268,7 +6268,7 @@
         <v>3.21</v>
       </c>
       <c r="M116" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N116" s="3">
         <v>14.52</v>
@@ -6318,7 +6318,7 @@
         <v>3.79</v>
       </c>
       <c r="M117" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N117" s="3">
         <v>16.240000000000002</v>
@@ -6368,7 +6368,7 @@
         <v>4.37</v>
       </c>
       <c r="M118" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N118" s="3">
         <v>17.97</v>
@@ -6418,7 +6418,7 @@
         <v>4.95</v>
       </c>
       <c r="M119" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N119" s="3">
         <v>19.7</v>
@@ -6468,7 +6468,7 @@
         <v>5.55</v>
       </c>
       <c r="M120" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N120" s="3">
         <v>21.51</v>
@@ -6518,7 +6518,7 @@
         <v>6.29</v>
       </c>
       <c r="M121" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N121" s="3">
         <v>23.729999999999997</v>
@@ -6568,7 +6568,7 @@
         <v>6.97</v>
       </c>
       <c r="M122" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N122" s="3">
         <v>25.77</v>
@@ -6618,7 +6618,7 @@
         <v>7.59</v>
       </c>
       <c r="M123" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N123" s="3">
         <v>27.62</v>
@@ -6668,7 +6668,7 @@
         <v>8.16</v>
       </c>
       <c r="M124" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N124" s="3">
         <v>29.319999999999997</v>
@@ -6718,7 +6718,7 @@
         <v>13.32</v>
       </c>
       <c r="M125" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N125" s="3">
         <v>31</v>
@@ -6732,7 +6732,7 @@
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B126" s="3">
         <v>0</v>
@@ -6768,7 +6768,7 @@
         <v>0.3</v>
       </c>
       <c r="M126" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N126" s="3">
         <v>5.45</v>
@@ -6782,7 +6782,7 @@
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B127" s="3">
         <v>1</v>
@@ -6818,7 +6818,7 @@
         <v>0.4</v>
       </c>
       <c r="M127" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N127" s="3">
         <v>6.9700000000000006</v>
@@ -6832,7 +6832,7 @@
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B128" s="3">
         <v>2</v>
@@ -6868,7 +6868,7 @@
         <v>0.49</v>
       </c>
       <c r="M128" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N128" s="3">
         <v>8.3899999999999988</v>
@@ -6882,7 +6882,7 @@
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B129" s="3">
         <v>3</v>
@@ -6918,7 +6918,7 @@
         <v>0.63</v>
       </c>
       <c r="M129" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N129" s="3">
         <v>9.4300000000000015</v>
@@ -6932,7 +6932,7 @@
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B130" s="3">
         <v>4</v>
@@ -6968,7 +6968,7 @@
         <v>0.77</v>
       </c>
       <c r="M130" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N130" s="3">
         <v>10.51</v>
@@ -6982,7 +6982,7 @@
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B131" s="3">
         <v>5</v>
@@ -7018,7 +7018,7 @@
         <v>0.9</v>
       </c>
       <c r="M131" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N131" s="3">
         <v>11.51</v>
@@ -7032,7 +7032,7 @@
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B132" s="3">
         <v>6</v>
@@ -7068,7 +7068,7 @@
         <v>1.04</v>
       </c>
       <c r="M132" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N132" s="3">
         <v>12.509999999999998</v>
@@ -7082,7 +7082,7 @@
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B133" s="3">
         <v>7</v>
@@ -7118,7 +7118,7 @@
         <v>1.17</v>
       </c>
       <c r="M133" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N133" s="3">
         <v>13.54</v>
@@ -7132,7 +7132,7 @@
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B134" s="3">
         <v>8</v>
@@ -7168,7 +7168,7 @@
         <v>1.31</v>
       </c>
       <c r="M134" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N134" s="3">
         <v>14.58</v>
@@ -7182,7 +7182,7 @@
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B135" s="3">
         <v>9</v>
@@ -7218,7 +7218,7 @@
         <v>1.45</v>
       </c>
       <c r="M135" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N135" s="3">
         <v>15.62</v>
@@ -7232,7 +7232,7 @@
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B136" s="3">
         <v>10</v>
@@ -7268,7 +7268,7 @@
         <v>1.58</v>
       </c>
       <c r="M136" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N136" s="3">
         <v>16.649999999999999</v>
@@ -7282,7 +7282,7 @@
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B137" s="3">
         <v>11</v>
@@ -7318,7 +7318,7 @@
         <v>1.72</v>
       </c>
       <c r="M137" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N137" s="3">
         <v>17.689999999999998</v>
@@ -7332,7 +7332,7 @@
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B138" s="3">
         <v>12</v>
@@ -7368,7 +7368,7 @@
         <v>1.85</v>
       </c>
       <c r="M138" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N138" s="3">
         <v>18.720000000000002</v>
@@ -7382,7 +7382,7 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B139" s="3">
         <v>13</v>
@@ -7418,7 +7418,7 @@
         <v>2.06</v>
       </c>
       <c r="M139" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N139" s="3">
         <v>19.86</v>
@@ -7432,7 +7432,7 @@
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B140" s="3">
         <v>14</v>
@@ -7468,7 +7468,7 @@
         <v>2.33</v>
       </c>
       <c r="M140" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N140" s="3">
         <v>21.11</v>
@@ -7482,7 +7482,7 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B141" s="3">
         <v>15</v>
@@ -7518,7 +7518,7 @@
         <v>2.6</v>
       </c>
       <c r="M141" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N141" s="3">
         <v>22.350000000000005</v>
@@ -7532,7 +7532,7 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B142" s="3">
         <v>16</v>
@@ -7568,7 +7568,7 @@
         <v>2.87</v>
       </c>
       <c r="M142" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N142" s="3">
         <v>23.610000000000003</v>
@@ -7582,7 +7582,7 @@
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B143" s="3">
         <v>17</v>
@@ -7618,7 +7618,7 @@
         <v>3.14</v>
       </c>
       <c r="M143" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N143" s="3">
         <v>24.840000000000003</v>
@@ -7632,7 +7632,7 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B144" s="3">
         <v>18</v>
@@ -7668,7 +7668,7 @@
         <v>3.41</v>
       </c>
       <c r="M144" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N144" s="3">
         <v>26.08</v>
@@ -7682,7 +7682,7 @@
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B145" s="3">
         <v>19</v>
@@ -7718,7 +7718,7 @@
         <v>3.69</v>
       </c>
       <c r="M145" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N145" s="3">
         <v>27.36</v>
@@ -7732,7 +7732,7 @@
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B146" s="3">
         <v>20</v>
@@ -7768,7 +7768,7 @@
         <v>3.96</v>
       </c>
       <c r="M146" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N146" s="3">
         <v>28.59</v>
@@ -7782,7 +7782,7 @@
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B147" s="3">
         <v>21</v>
@@ -7818,7 +7818,7 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="M147" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N147" s="3">
         <v>29.84</v>
@@ -7832,7 +7832,7 @@
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B148" s="3">
         <v>22</v>
@@ -7868,7 +7868,7 @@
         <v>4.5</v>
       </c>
       <c r="M148" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N148" s="3">
         <v>31.090000000000003</v>
@@ -7882,7 +7882,7 @@
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B149" s="3">
         <v>23</v>
@@ -7918,7 +7918,7 @@
         <v>4.7699999999999996</v>
       </c>
       <c r="M149" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N149" s="3">
         <v>32.339999999999996</v>
@@ -7932,7 +7932,7 @@
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B150" s="3">
         <v>24</v>
@@ -7968,7 +7968,7 @@
         <v>5.04</v>
       </c>
       <c r="M150" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N150" s="3">
         <v>33.57</v>
@@ -7982,7 +7982,7 @@
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B151" s="3">
         <v>25</v>
@@ -8018,7 +8018,7 @@
         <v>5.31</v>
       </c>
       <c r="M151" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N151" s="3">
         <v>34.830000000000005</v>
@@ -8032,7 +8032,7 @@
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B152" s="3">
         <v>26</v>
@@ -8068,7 +8068,7 @@
         <v>5.59</v>
       </c>
       <c r="M152" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N152" s="3">
         <v>36.099999999999994</v>
@@ -8082,7 +8082,7 @@
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B153" s="3">
         <v>27</v>
@@ -8118,7 +8118,7 @@
         <v>5.86</v>
       </c>
       <c r="M153" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N153" s="3">
         <v>37.32</v>
@@ -8132,7 +8132,7 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B154" s="3">
         <v>28</v>
@@ -8168,7 +8168,7 @@
         <v>6.13</v>
       </c>
       <c r="M154" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N154" s="3">
         <v>38.590000000000011</v>
@@ -8182,7 +8182,7 @@
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B155" s="3">
         <v>29</v>
@@ -8218,7 +8218,7 @@
         <v>6.48</v>
       </c>
       <c r="M155" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N155" s="3">
         <v>39.870000000000005</v>
@@ -8232,7 +8232,7 @@
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B156" s="3">
         <v>30</v>
@@ -8268,7 +8268,7 @@
         <v>6.93</v>
       </c>
       <c r="M156" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N156" s="3">
         <v>41.209999999999994</v>
@@ -8282,7 +8282,7 @@
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B157" s="3">
         <v>0</v>
@@ -8318,7 +8318,7 @@
         <v>0.3</v>
       </c>
       <c r="M157" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N157" s="3">
         <v>5.45</v>
@@ -8332,7 +8332,7 @@
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B158" s="3">
         <v>1</v>
@@ -8368,7 +8368,7 @@
         <v>0.4</v>
       </c>
       <c r="M158" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N158" s="3">
         <v>6.9700000000000006</v>
@@ -8382,7 +8382,7 @@
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B159" s="3">
         <v>2</v>
@@ -8418,7 +8418,7 @@
         <v>0.49</v>
       </c>
       <c r="M159" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N159" s="3">
         <v>8.3899999999999988</v>
@@ -8432,7 +8432,7 @@
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B160" s="3">
         <v>3</v>
@@ -8468,7 +8468,7 @@
         <v>0.63</v>
       </c>
       <c r="M160" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N160" s="3">
         <v>9.4300000000000015</v>
@@ -8482,7 +8482,7 @@
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B161" s="3">
         <v>4</v>
@@ -8518,7 +8518,7 @@
         <v>0.77</v>
       </c>
       <c r="M161" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N161" s="3">
         <v>10.51</v>
@@ -8532,7 +8532,7 @@
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B162" s="3">
         <v>5</v>
@@ -8568,7 +8568,7 @@
         <v>0.9</v>
       </c>
       <c r="M162" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N162" s="3">
         <v>11.51</v>
@@ -8582,7 +8582,7 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B163" s="3">
         <v>6</v>
@@ -8618,7 +8618,7 @@
         <v>1.04</v>
       </c>
       <c r="M163" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N163" s="3">
         <v>12.509999999999998</v>
@@ -8632,7 +8632,7 @@
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B164" s="3">
         <v>7</v>
@@ -8668,7 +8668,7 @@
         <v>1.17</v>
       </c>
       <c r="M164" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N164" s="3">
         <v>13.54</v>
@@ -8682,7 +8682,7 @@
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B165" s="3">
         <v>8</v>
@@ -8718,7 +8718,7 @@
         <v>1.31</v>
       </c>
       <c r="M165" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N165" s="3">
         <v>14.58</v>
@@ -8732,7 +8732,7 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B166" s="3">
         <v>9</v>
@@ -8768,7 +8768,7 @@
         <v>1.45</v>
       </c>
       <c r="M166" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N166" s="3">
         <v>15.62</v>
@@ -8782,7 +8782,7 @@
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B167" s="3">
         <v>10</v>
@@ -8818,7 +8818,7 @@
         <v>1.58</v>
       </c>
       <c r="M167" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N167" s="3">
         <v>16.649999999999999</v>
@@ -8832,7 +8832,7 @@
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B168" s="3">
         <v>11</v>
@@ -8868,7 +8868,7 @@
         <v>1.72</v>
       </c>
       <c r="M168" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N168" s="3">
         <v>17.689999999999998</v>
@@ -8882,7 +8882,7 @@
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B169" s="3">
         <v>12</v>
@@ -8918,7 +8918,7 @@
         <v>1.85</v>
       </c>
       <c r="M169" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N169" s="3">
         <v>18.720000000000002</v>
@@ -8932,7 +8932,7 @@
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B170" s="3">
         <v>13</v>
@@ -8968,7 +8968,7 @@
         <v>2.06</v>
       </c>
       <c r="M170" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N170" s="3">
         <v>19.86</v>
@@ -8982,7 +8982,7 @@
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B171" s="3">
         <v>14</v>
@@ -9018,7 +9018,7 @@
         <v>2.33</v>
       </c>
       <c r="M171" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N171" s="3">
         <v>21.11</v>
@@ -9032,7 +9032,7 @@
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B172" s="3">
         <v>15</v>
@@ -9068,7 +9068,7 @@
         <v>2.6</v>
       </c>
       <c r="M172" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N172" s="3">
         <v>22.350000000000005</v>
@@ -9082,7 +9082,7 @@
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B173" s="3">
         <v>16</v>
@@ -9118,7 +9118,7 @@
         <v>0.3</v>
       </c>
       <c r="M173" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N173" s="3">
         <v>5.45</v>
@@ -9132,7 +9132,7 @@
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B174" s="3">
         <v>17</v>
@@ -9168,7 +9168,7 @@
         <v>0.4</v>
       </c>
       <c r="M174" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N174" s="3">
         <v>6.9700000000000006</v>
@@ -9182,7 +9182,7 @@
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B175" s="3">
         <v>18</v>
@@ -9218,7 +9218,7 @@
         <v>0.49</v>
       </c>
       <c r="M175" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N175" s="3">
         <v>8.3899999999999988</v>
@@ -9232,7 +9232,7 @@
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B176" s="3">
         <v>19</v>
@@ -9268,7 +9268,7 @@
         <v>0.63</v>
       </c>
       <c r="M176" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N176" s="3">
         <v>9.4300000000000015</v>
@@ -9282,7 +9282,7 @@
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B177" s="3">
         <v>20</v>
@@ -9318,7 +9318,7 @@
         <v>0.77</v>
       </c>
       <c r="M177" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N177" s="3">
         <v>10.51</v>
@@ -9332,7 +9332,7 @@
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B178" s="3">
         <v>21</v>
@@ -9368,7 +9368,7 @@
         <v>0.9</v>
       </c>
       <c r="M178" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N178" s="3">
         <v>11.51</v>
@@ -9382,7 +9382,7 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B179" s="3">
         <v>22</v>
@@ -9418,7 +9418,7 @@
         <v>1.04</v>
       </c>
       <c r="M179" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N179" s="3">
         <v>12.509999999999998</v>
@@ -9432,7 +9432,7 @@
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B180" s="3">
         <v>23</v>
@@ -9468,7 +9468,7 @@
         <v>1.17</v>
       </c>
       <c r="M180" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N180" s="3">
         <v>13.54</v>
@@ -9482,7 +9482,7 @@
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B181" s="3">
         <v>24</v>
@@ -9518,7 +9518,7 @@
         <v>1.31</v>
       </c>
       <c r="M181" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N181" s="3">
         <v>14.58</v>
@@ -9532,7 +9532,7 @@
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B182" s="3">
         <v>25</v>
@@ -9568,7 +9568,7 @@
         <v>1.45</v>
       </c>
       <c r="M182" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N182" s="3">
         <v>15.62</v>
@@ -9582,7 +9582,7 @@
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B183" s="3">
         <v>26</v>
@@ -9618,7 +9618,7 @@
         <v>1.58</v>
       </c>
       <c r="M183" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N183" s="3">
         <v>16.649999999999999</v>
@@ -9632,7 +9632,7 @@
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B184" s="3">
         <v>27</v>
@@ -9668,7 +9668,7 @@
         <v>1.72</v>
       </c>
       <c r="M184" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N184" s="3">
         <v>17.689999999999998</v>
@@ -9682,7 +9682,7 @@
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B185" s="3">
         <v>28</v>
@@ -9718,7 +9718,7 @@
         <v>1.85</v>
       </c>
       <c r="M185" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N185" s="3">
         <v>18.720000000000002</v>
@@ -9732,7 +9732,7 @@
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B186" s="3">
         <v>29</v>
@@ -9768,7 +9768,7 @@
         <v>2.06</v>
       </c>
       <c r="M186" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N186" s="3">
         <v>19.86</v>
@@ -9782,7 +9782,7 @@
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B187" s="3">
         <v>30</v>
@@ -9818,7 +9818,7 @@
         <v>2.33</v>
       </c>
       <c r="M187" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N187" s="3">
         <v>21.11</v>
@@ -9832,7 +9832,7 @@
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B188" s="3">
         <v>0</v>
@@ -9868,7 +9868,7 @@
         <v>0.51</v>
       </c>
       <c r="M188" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N188" s="3">
         <v>6.28</v>
@@ -9882,7 +9882,7 @@
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B189" s="3">
         <v>1</v>
@@ -9918,7 +9918,7 @@
         <v>0.6</v>
       </c>
       <c r="M189" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N189" s="3">
         <v>7.4599999999999991</v>
@@ -9932,7 +9932,7 @@
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B190" s="3">
         <v>2</v>
@@ -9968,7 +9968,7 @@
         <v>0.7</v>
       </c>
       <c r="M190" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N190" s="3">
         <v>9.1000000000000014</v>
@@ -9982,7 +9982,7 @@
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B191" s="3">
         <v>3</v>
@@ -10018,7 +10018,7 @@
         <v>0.81</v>
       </c>
       <c r="M191" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N191" s="3">
         <v>9.5400000000000009</v>
@@ -10032,7 +10032,7 @@
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B192" s="3">
         <v>4</v>
@@ -10068,7 +10068,7 @@
         <v>0.96</v>
       </c>
       <c r="M192" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N192" s="3">
         <v>9.870000000000001</v>
@@ -10082,7 +10082,7 @@
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B193" s="3">
         <v>5</v>
@@ -10118,7 +10118,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="M193" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N193" s="3">
         <v>10.199999999999999</v>
@@ -10132,7 +10132,7 @@
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B194" s="3">
         <v>6</v>
@@ -10168,7 +10168,7 @@
         <v>1.22</v>
       </c>
       <c r="M194" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N194" s="3">
         <v>10.5</v>
@@ -10182,7 +10182,7 @@
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B195" s="3">
         <v>7</v>
@@ -10218,7 +10218,7 @@
         <v>1.34</v>
       </c>
       <c r="M195" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N195" s="3">
         <v>10.79</v>
@@ -10232,7 +10232,7 @@
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B196" s="3">
         <v>8</v>
@@ -10268,7 +10268,7 @@
         <v>1.44</v>
       </c>
       <c r="M196" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N196" s="3">
         <v>11.04</v>
@@ -10282,7 +10282,7 @@
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B197" s="3">
         <v>9</v>
@@ -10318,7 +10318,7 @@
         <v>1.54</v>
       </c>
       <c r="M197" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N197" s="3">
         <v>11.280000000000001</v>
@@ -10332,7 +10332,7 @@
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B198" s="3">
         <v>10</v>
@@ -10368,7 +10368,7 @@
         <v>1.65</v>
       </c>
       <c r="M198" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N198" s="3">
         <v>11.49</v>
@@ -10382,7 +10382,7 @@
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B199" s="3">
         <v>11</v>
@@ -10418,7 +10418,7 @@
         <v>1.72</v>
       </c>
       <c r="M199" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N199" s="3">
         <v>11.68</v>
@@ -10432,7 +10432,7 @@
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B200" s="3">
         <v>12</v>
@@ -10468,7 +10468,7 @@
         <v>1.79</v>
       </c>
       <c r="M200" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N200" s="3">
         <v>11.86</v>
@@ -10482,7 +10482,7 @@
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B201" s="3">
         <v>13</v>
@@ -10518,7 +10518,7 @@
         <v>1.86</v>
       </c>
       <c r="M201" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N201" s="3">
         <v>12.009999999999998</v>
@@ -10532,7 +10532,7 @@
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B202" s="3">
         <v>14</v>
@@ -10568,7 +10568,7 @@
         <v>1.92</v>
       </c>
       <c r="M202" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N202" s="3">
         <v>12.17</v>
@@ -10582,7 +10582,7 @@
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B203" s="3">
         <v>15</v>
@@ -10618,7 +10618,7 @@
         <v>1.98</v>
       </c>
       <c r="M203" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N203" s="3">
         <v>12.31</v>
@@ -10632,7 +10632,7 @@
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B204" s="3">
         <v>16</v>
@@ -10668,7 +10668,7 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="M204" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N204" s="3">
         <v>12.430000000000001</v>
@@ -10682,7 +10682,7 @@
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B205" s="3">
         <v>17</v>
@@ -10718,7 +10718,7 @@
         <v>2.08</v>
       </c>
       <c r="M205" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N205" s="3">
         <v>12.55</v>
@@ -10732,7 +10732,7 @@
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B206" s="3">
         <v>18</v>
@@ -10768,7 +10768,7 @@
         <v>2.13</v>
       </c>
       <c r="M206" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N206" s="3">
         <v>12.669999999999998</v>
@@ -10782,7 +10782,7 @@
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B207" s="3">
         <v>19</v>
@@ -10818,7 +10818,7 @@
         <v>2.17</v>
       </c>
       <c r="M207" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N207" s="3">
         <v>12.76</v>
@@ -10832,7 +10832,7 @@
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B208" s="3">
         <v>20</v>
@@ -10868,7 +10868,7 @@
         <v>2.21</v>
       </c>
       <c r="M208" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N208" s="3">
         <v>12.86</v>
@@ -10882,7 +10882,7 @@
     </row>
     <row r="209" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B209" s="3">
         <v>21</v>
@@ -10918,7 +10918,7 @@
         <v>2.25</v>
       </c>
       <c r="M209" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N209" s="3">
         <v>12.96</v>
@@ -10932,7 +10932,7 @@
     </row>
     <row r="210" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B210" s="3">
         <v>22</v>
@@ -10968,7 +10968,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="M210" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N210" s="3">
         <v>13.030000000000001</v>
@@ -10982,7 +10982,7 @@
     </row>
     <row r="211" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B211" s="3">
         <v>23</v>
@@ -11018,7 +11018,7 @@
         <v>2.31</v>
       </c>
       <c r="M211" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N211" s="3">
         <v>13.090000000000002</v>
@@ -11032,7 +11032,7 @@
     </row>
     <row r="212" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B212" s="3">
         <v>24</v>
@@ -11068,7 +11068,7 @@
         <v>2.34</v>
       </c>
       <c r="M212" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N212" s="3">
         <v>13.16</v>
@@ -11082,7 +11082,7 @@
     </row>
     <row r="213" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B213" s="3">
         <v>25</v>
@@ -11118,7 +11118,7 @@
         <v>2.37</v>
       </c>
       <c r="M213" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N213" s="3">
         <v>13.239999999999998</v>
@@ -11132,7 +11132,7 @@
     </row>
     <row r="214" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B214" s="3">
         <v>26</v>
@@ -11168,7 +11168,7 @@
         <v>2.4</v>
       </c>
       <c r="M214" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N214" s="3">
         <v>13.309999999999999</v>
@@ -11182,7 +11182,7 @@
     </row>
     <row r="215" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B215" s="3">
         <v>27</v>
@@ -11218,7 +11218,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="M215" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N215" s="3">
         <v>13.379999999999999</v>
@@ -11232,7 +11232,7 @@
     </row>
     <row r="216" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B216" s="3">
         <v>28</v>
@@ -11268,7 +11268,7 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="M216" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N216" s="3">
         <v>13.419999999999998</v>
@@ -11282,7 +11282,7 @@
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B217" s="3">
         <v>29</v>
@@ -11318,7 +11318,7 @@
         <v>2.4700000000000002</v>
       </c>
       <c r="M217" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N217" s="3">
         <v>13.48</v>
@@ -11332,7 +11332,7 @@
     </row>
     <row r="218" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B218" s="3">
         <v>30</v>
@@ -11368,7 +11368,7 @@
         <v>2.5</v>
       </c>
       <c r="M218" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N218" s="3">
         <v>13.54</v>
@@ -11382,7 +11382,7 @@
     </row>
     <row r="219" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B219" s="3">
         <v>0</v>
@@ -11418,7 +11418,7 @@
         <v>0.51</v>
       </c>
       <c r="M219" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N219" s="3">
         <v>6.28</v>
@@ -11432,7 +11432,7 @@
     </row>
     <row r="220" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B220" s="3">
         <v>1</v>
@@ -11468,7 +11468,7 @@
         <v>0.6</v>
       </c>
       <c r="M220" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N220" s="3">
         <v>7.4599999999999991</v>
@@ -11482,7 +11482,7 @@
     </row>
     <row r="221" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B221" s="3">
         <v>2</v>
@@ -11518,7 +11518,7 @@
         <v>0.7</v>
       </c>
       <c r="M221" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N221" s="3">
         <v>9.1000000000000014</v>
@@ -11532,7 +11532,7 @@
     </row>
     <row r="222" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B222" s="3">
         <v>3</v>
@@ -11568,7 +11568,7 @@
         <v>0.81</v>
       </c>
       <c r="M222" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N222" s="3">
         <v>9.5400000000000009</v>
@@ -11582,7 +11582,7 @@
     </row>
     <row r="223" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B223" s="3">
         <v>4</v>
@@ -11618,7 +11618,7 @@
         <v>0.96</v>
       </c>
       <c r="M223" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N223" s="3">
         <v>9.870000000000001</v>
@@ -11632,7 +11632,7 @@
     </row>
     <row r="224" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B224" s="3">
         <v>5</v>
@@ -11668,7 +11668,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="M224" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N224" s="3">
         <v>10.199999999999999</v>
@@ -11682,7 +11682,7 @@
     </row>
     <row r="225" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B225" s="3">
         <v>6</v>
@@ -11718,7 +11718,7 @@
         <v>1.22</v>
       </c>
       <c r="M225" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N225" s="3">
         <v>10.5</v>
@@ -11732,7 +11732,7 @@
     </row>
     <row r="226" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B226" s="3">
         <v>7</v>
@@ -11768,7 +11768,7 @@
         <v>1.34</v>
       </c>
       <c r="M226" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N226" s="3">
         <v>10.79</v>
@@ -11782,7 +11782,7 @@
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B227" s="3">
         <v>8</v>
@@ -11818,7 +11818,7 @@
         <v>1.44</v>
       </c>
       <c r="M227" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N227" s="3">
         <v>11.04</v>
@@ -11832,7 +11832,7 @@
     </row>
     <row r="228" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B228" s="3">
         <v>9</v>
@@ -11868,7 +11868,7 @@
         <v>1.54</v>
       </c>
       <c r="M228" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N228" s="3">
         <v>11.280000000000001</v>
@@ -11882,7 +11882,7 @@
     </row>
     <row r="229" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B229" s="3">
         <v>10</v>
@@ -11918,7 +11918,7 @@
         <v>1.65</v>
       </c>
       <c r="M229" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N229" s="3">
         <v>11.49</v>
@@ -11932,7 +11932,7 @@
     </row>
     <row r="230" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B230" s="3">
         <v>11</v>
@@ -11968,7 +11968,7 @@
         <v>1.72</v>
       </c>
       <c r="M230" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N230" s="3">
         <v>11.68</v>
@@ -11982,7 +11982,7 @@
     </row>
     <row r="231" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B231" s="3">
         <v>12</v>
@@ -12018,7 +12018,7 @@
         <v>1.79</v>
       </c>
       <c r="M231" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N231" s="3">
         <v>11.86</v>
@@ -12032,7 +12032,7 @@
     </row>
     <row r="232" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B232" s="3">
         <v>13</v>
@@ -12068,7 +12068,7 @@
         <v>1.86</v>
       </c>
       <c r="M232" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N232" s="3">
         <v>12.009999999999998</v>
@@ -12082,7 +12082,7 @@
     </row>
     <row r="233" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B233" s="3">
         <v>14</v>
@@ -12118,7 +12118,7 @@
         <v>1.92</v>
       </c>
       <c r="M233" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N233" s="3">
         <v>12.17</v>
@@ -12132,7 +12132,7 @@
     </row>
     <row r="234" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B234" s="3">
         <v>15</v>
@@ -12168,7 +12168,7 @@
         <v>1.98</v>
       </c>
       <c r="M234" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N234" s="3">
         <v>12.31</v>
@@ -12182,7 +12182,7 @@
     </row>
     <row r="235" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B235" s="3">
         <v>16</v>
@@ -12218,7 +12218,7 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="M235" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N235" s="3">
         <v>12.430000000000001</v>
@@ -12232,7 +12232,7 @@
     </row>
     <row r="236" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B236" s="3">
         <v>17</v>
@@ -12268,7 +12268,7 @@
         <v>2.08</v>
       </c>
       <c r="M236" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N236" s="3">
         <v>6.28</v>
@@ -12282,7 +12282,7 @@
     </row>
     <row r="237" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B237" s="3">
         <v>18</v>
@@ -12318,7 +12318,7 @@
         <v>0.6</v>
       </c>
       <c r="M237" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N237" s="3">
         <v>7.4599999999999991</v>
@@ -12332,7 +12332,7 @@
     </row>
     <row r="238" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B238" s="3">
         <v>19</v>
@@ -12368,7 +12368,7 @@
         <v>0.7</v>
       </c>
       <c r="M238" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N238" s="3">
         <v>9.1000000000000014</v>
@@ -12382,7 +12382,7 @@
     </row>
     <row r="239" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B239" s="3">
         <v>20</v>
@@ -12418,7 +12418,7 @@
         <v>0.81</v>
       </c>
       <c r="M239" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N239" s="3">
         <v>9.5400000000000009</v>
@@ -12432,7 +12432,7 @@
     </row>
     <row r="240" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B240" s="3">
         <v>21</v>
@@ -12468,7 +12468,7 @@
         <v>0.96</v>
       </c>
       <c r="M240" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N240" s="3">
         <v>9.870000000000001</v>
@@ -12482,7 +12482,7 @@
     </row>
     <row r="241" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B241" s="3">
         <v>22</v>
@@ -12518,7 +12518,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="M241" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N241" s="3">
         <v>10.199999999999999</v>
@@ -12532,7 +12532,7 @@
     </row>
     <row r="242" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B242" s="3">
         <v>23</v>
@@ -12568,7 +12568,7 @@
         <v>1.22</v>
       </c>
       <c r="M242" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N242" s="3">
         <v>10.5</v>
@@ -12582,7 +12582,7 @@
     </row>
     <row r="243" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B243" s="3">
         <v>24</v>
@@ -12618,7 +12618,7 @@
         <v>1.34</v>
       </c>
       <c r="M243" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N243" s="3">
         <v>10.79</v>
@@ -12632,7 +12632,7 @@
     </row>
     <row r="244" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B244" s="3">
         <v>25</v>
@@ -12668,7 +12668,7 @@
         <v>1.44</v>
       </c>
       <c r="M244" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N244" s="3">
         <v>11.04</v>
@@ -12682,7 +12682,7 @@
     </row>
     <row r="245" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B245" s="3">
         <v>26</v>
@@ -12718,7 +12718,7 @@
         <v>1.54</v>
       </c>
       <c r="M245" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N245" s="3">
         <v>11.280000000000001</v>
@@ -12732,7 +12732,7 @@
     </row>
     <row r="246" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B246" s="3">
         <v>27</v>
@@ -12768,7 +12768,7 @@
         <v>1.65</v>
       </c>
       <c r="M246" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N246" s="3">
         <v>11.49</v>
@@ -12782,7 +12782,7 @@
     </row>
     <row r="247" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B247" s="3">
         <v>28</v>
@@ -12818,7 +12818,7 @@
         <v>1.72</v>
       </c>
       <c r="M247" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N247" s="3">
         <v>11.68</v>
@@ -12832,7 +12832,7 @@
     </row>
     <row r="248" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B248" s="3">
         <v>29</v>
@@ -12868,7 +12868,7 @@
         <v>1.79</v>
       </c>
       <c r="M248" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N248" s="3">
         <v>11.86</v>
@@ -12882,7 +12882,7 @@
     </row>
     <row r="249" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B249" s="3">
         <v>30</v>
@@ -12918,7 +12918,7 @@
         <v>1.86</v>
       </c>
       <c r="M249" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N249" s="3">
         <v>12.009999999999998</v>
@@ -12932,7 +12932,7 @@
     </row>
     <row r="250" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B250" s="3">
         <v>0</v>
@@ -12965,7 +12965,7 @@
         <v>0.82</v>
       </c>
       <c r="M250" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N250" s="3">
         <v>6.75</v>
@@ -12979,7 +12979,7 @@
     </row>
     <row r="251" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B251" s="3">
         <v>1</v>
@@ -13015,7 +13015,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="M251" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N251" s="3">
         <v>17.079999999999998</v>
@@ -13029,7 +13029,7 @@
     </row>
     <row r="252" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B252" s="3">
         <v>2</v>
@@ -13065,7 +13065,7 @@
         <v>1.67</v>
       </c>
       <c r="M252" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N252" s="3">
         <v>11.78</v>
@@ -13079,7 +13079,7 @@
     </row>
     <row r="253" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B253" s="3">
         <v>3</v>
@@ -13115,7 +13115,7 @@
         <v>2.38</v>
       </c>
       <c r="M253" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N253" s="3">
         <v>14.48</v>
@@ -13129,7 +13129,7 @@
     </row>
     <row r="254" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B254" s="3">
         <v>4</v>
@@ -13165,7 +13165,7 @@
         <v>3.1</v>
       </c>
       <c r="M254" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N254" s="3">
         <v>17.22</v>
@@ -13179,7 +13179,7 @@
     </row>
     <row r="255" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B255" s="3">
         <v>5</v>
@@ -13215,7 +13215,7 @@
         <v>3.82</v>
       </c>
       <c r="M255" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N255" s="3">
         <v>19.940000000000001</v>
@@ -13229,7 +13229,7 @@
     </row>
     <row r="256" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B256" s="3">
         <v>6</v>
@@ -13265,7 +13265,7 @@
         <v>4.54</v>
       </c>
       <c r="M256" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N256" s="3">
         <v>22.669999999999998</v>
@@ -13279,7 +13279,7 @@
     </row>
     <row r="257" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B257" s="3">
         <v>7</v>
@@ -13315,7 +13315,7 @@
         <v>5.26</v>
       </c>
       <c r="M257" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N257" s="3">
         <v>25.39</v>
@@ -13329,7 +13329,7 @@
     </row>
     <row r="258" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B258" s="3">
         <v>8</v>
@@ -13365,7 +13365,7 @@
         <v>5.98</v>
       </c>
       <c r="M258" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N258" s="3">
         <v>28.11</v>
@@ -13379,7 +13379,7 @@
     </row>
     <row r="259" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B259" s="3">
         <v>9</v>
@@ -13415,7 +13415,7 @@
         <v>6.7</v>
       </c>
       <c r="M259" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N259" s="3">
         <v>30.839999999999996</v>
@@ -13429,7 +13429,7 @@
     </row>
     <row r="260" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B260" s="3">
         <v>10</v>
@@ -13465,7 +13465,7 @@
         <v>7.56</v>
       </c>
       <c r="M260" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N260" s="3">
         <v>33.809999999999995</v>
@@ -13479,7 +13479,7 @@
     </row>
     <row r="261" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B261" s="3">
         <v>11</v>
@@ -13515,7 +13515,7 @@
         <v>8.7799999999999994</v>
       </c>
       <c r="M261" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N261" s="3">
         <v>37.440000000000005</v>
@@ -13529,7 +13529,7 @@
     </row>
     <row r="262" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B262" s="3">
         <v>12</v>
@@ -13565,7 +13565,7 @@
         <v>10</v>
       </c>
       <c r="M262" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N262" s="3">
         <v>41.05</v>
@@ -13579,7 +13579,7 @@
     </row>
     <row r="263" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B263" s="3">
         <v>13</v>
@@ -13615,7 +13615,7 @@
         <v>11.22</v>
       </c>
       <c r="M263" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N263" s="3">
         <v>44.689999999999991</v>
@@ -13629,7 +13629,7 @@
     </row>
     <row r="264" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B264" s="3">
         <v>14</v>
@@ -13665,7 +13665,7 @@
         <v>12.45</v>
       </c>
       <c r="M264" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N264" s="3">
         <v>48.319999999999993</v>
@@ -13679,7 +13679,7 @@
     </row>
     <row r="265" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B265" s="3">
         <v>15</v>
@@ -13715,7 +13715,7 @@
         <v>13.67</v>
       </c>
       <c r="M265" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N265" s="3">
         <v>51.94</v>
@@ -13729,7 +13729,7 @@
     </row>
     <row r="266" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B266" s="3">
         <v>16</v>
@@ -13765,7 +13765,7 @@
         <v>14.99</v>
       </c>
       <c r="M266" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N266" s="3">
         <v>55.67</v>
@@ -13779,7 +13779,7 @@
     </row>
     <row r="267" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B267" s="3">
         <v>17</v>
@@ -13815,7 +13815,7 @@
         <v>16.11</v>
       </c>
       <c r="M267" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N267" s="3">
         <v>59.180000000000007</v>
@@ -13829,7 +13829,7 @@
     </row>
     <row r="268" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B268" s="3">
         <v>18</v>
@@ -13865,7 +13865,7 @@
         <v>17.329999999999998</v>
       </c>
       <c r="M268" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N268" s="3">
         <v>62.809999999999995</v>
@@ -13879,7 +13879,7 @@
     </row>
     <row r="269" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B269" s="3">
         <v>19</v>
@@ -13915,7 +13915,7 @@
         <v>18.55</v>
       </c>
       <c r="M269" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N269" s="3">
         <v>66.45</v>
@@ -13929,7 +13929,7 @@
     </row>
     <row r="270" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B270" s="3">
         <v>20</v>
@@ -13965,7 +13965,7 @@
         <v>19.77</v>
       </c>
       <c r="M270" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N270" s="3">
         <v>70.05</v>
@@ -13979,7 +13979,7 @@
     </row>
     <row r="271" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B271" s="3">
         <v>21</v>
@@ -14015,7 +14015,7 @@
         <v>21</v>
       </c>
       <c r="M271" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N271" s="3">
         <v>73.69</v>
@@ -14029,7 +14029,7 @@
     </row>
     <row r="272" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B272" s="3">
         <v>22</v>
@@ -14065,7 +14065,7 @@
         <v>22.22</v>
       </c>
       <c r="M272" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N272" s="3">
         <v>77.319999999999993</v>
@@ -14079,7 +14079,7 @@
     </row>
     <row r="273" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B273" s="3">
         <v>23</v>
@@ -14115,7 +14115,7 @@
         <v>23.74</v>
       </c>
       <c r="M273" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N273" s="3">
         <v>81.56</v>
@@ -14129,7 +14129,7 @@
     </row>
     <row r="274" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B274" s="3">
         <v>24</v>
@@ -14165,7 +14165,7 @@
         <v>25.34</v>
       </c>
       <c r="M274" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N274" s="3">
         <v>85.95</v>
@@ -14179,7 +14179,7 @@
     </row>
     <row r="275" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B275" s="3">
         <v>25</v>
@@ -14215,7 +14215,7 @@
         <v>26.95</v>
       </c>
       <c r="M275" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N275" s="3">
         <v>90.36</v>
@@ -14229,7 +14229,7 @@
     </row>
     <row r="276" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B276" s="3">
         <v>26</v>
@@ -14265,7 +14265,7 @@
         <v>28.73</v>
       </c>
       <c r="M276" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N276" s="3">
         <v>95.259999999999991</v>
@@ -14279,7 +14279,7 @@
     </row>
     <row r="277" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B277" s="3">
         <v>27</v>
@@ -14315,7 +14315,7 @@
         <v>30.51</v>
       </c>
       <c r="M277" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N277" s="3">
         <v>100.15</v>
@@ -14329,7 +14329,7 @@
     </row>
     <row r="278" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B278" s="3">
         <v>28</v>
@@ -14365,7 +14365,7 @@
         <v>31.85</v>
       </c>
       <c r="M278" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N278" s="3">
         <v>103.83000000000001</v>
@@ -14379,7 +14379,7 @@
     </row>
     <row r="279" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B279" s="3">
         <v>29</v>
@@ -14415,7 +14415,7 @@
         <v>33.630000000000003</v>
       </c>
       <c r="M279" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N279" s="3">
         <v>108.73000000000002</v>
@@ -14429,7 +14429,7 @@
     </row>
     <row r="280" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B280" s="3">
         <v>30</v>
@@ -14465,7 +14465,7 @@
         <v>34.97</v>
       </c>
       <c r="M280" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N280" s="3">
         <v>112.4</v>
@@ -14479,7 +14479,7 @@
     </row>
     <row r="281" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B281" s="3">
         <v>0</v>
@@ -14512,7 +14512,7 @@
         <v>0.82</v>
       </c>
       <c r="M281" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N281" s="3">
         <v>6.75</v>
@@ -14526,7 +14526,7 @@
     </row>
     <row r="282" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B282" s="3">
         <v>1</v>
@@ -14562,7 +14562,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="M282" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N282" s="3">
         <v>17.079999999999998</v>
@@ -14576,7 +14576,7 @@
     </row>
     <row r="283" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B283" s="3">
         <v>2</v>
@@ -14612,7 +14612,7 @@
         <v>1.67</v>
       </c>
       <c r="M283" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N283" s="3">
         <v>11.78</v>
@@ -14626,7 +14626,7 @@
     </row>
     <row r="284" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B284" s="3">
         <v>3</v>
@@ -14662,7 +14662,7 @@
         <v>2.38</v>
       </c>
       <c r="M284" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N284" s="3">
         <v>14.48</v>
@@ -14676,7 +14676,7 @@
     </row>
     <row r="285" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B285" s="3">
         <v>4</v>
@@ -14712,7 +14712,7 @@
         <v>3.1</v>
       </c>
       <c r="M285" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N285" s="3">
         <v>17.22</v>
@@ -14726,7 +14726,7 @@
     </row>
     <row r="286" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B286" s="3">
         <v>5</v>
@@ -14762,7 +14762,7 @@
         <v>3.82</v>
       </c>
       <c r="M286" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N286" s="3">
         <v>19.940000000000001</v>
@@ -14776,7 +14776,7 @@
     </row>
     <row r="287" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B287" s="3">
         <v>6</v>
@@ -14812,7 +14812,7 @@
         <v>4.54</v>
       </c>
       <c r="M287" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N287" s="3">
         <v>22.669999999999998</v>
@@ -14826,7 +14826,7 @@
     </row>
     <row r="288" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B288" s="3">
         <v>7</v>
@@ -14862,7 +14862,7 @@
         <v>5.26</v>
       </c>
       <c r="M288" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N288" s="3">
         <v>25.39</v>
@@ -14876,7 +14876,7 @@
     </row>
     <row r="289" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B289" s="3">
         <v>8</v>
@@ -14912,7 +14912,7 @@
         <v>5.98</v>
       </c>
       <c r="M289" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N289" s="3">
         <v>28.11</v>
@@ -14926,7 +14926,7 @@
     </row>
     <row r="290" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B290" s="3">
         <v>9</v>
@@ -14962,7 +14962,7 @@
         <v>6.7</v>
       </c>
       <c r="M290" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N290" s="3">
         <v>30.839999999999996</v>
@@ -14976,7 +14976,7 @@
     </row>
     <row r="291" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B291" s="3">
         <v>10</v>
@@ -15012,7 +15012,7 @@
         <v>7.56</v>
       </c>
       <c r="M291" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N291" s="3">
         <v>33.809999999999995</v>
@@ -15026,7 +15026,7 @@
     </row>
     <row r="292" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B292" s="3">
         <v>11</v>
@@ -15062,7 +15062,7 @@
         <v>8.7799999999999994</v>
       </c>
       <c r="M292" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N292" s="3">
         <v>37.440000000000005</v>
@@ -15076,7 +15076,7 @@
     </row>
     <row r="293" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B293" s="3">
         <v>12</v>
@@ -15112,7 +15112,7 @@
         <v>10</v>
       </c>
       <c r="M293" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N293" s="3">
         <v>41.05</v>
@@ -15126,7 +15126,7 @@
     </row>
     <row r="294" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B294" s="3">
         <v>13</v>
@@ -15162,7 +15162,7 @@
         <v>11.22</v>
       </c>
       <c r="M294" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N294" s="3">
         <v>44.689999999999991</v>
@@ -15176,7 +15176,7 @@
     </row>
     <row r="295" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B295" s="3">
         <v>14</v>
@@ -15212,7 +15212,7 @@
         <v>12.45</v>
       </c>
       <c r="M295" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N295" s="3">
         <v>48.319999999999993</v>
@@ -15226,7 +15226,7 @@
     </row>
     <row r="296" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B296" s="3">
         <v>15</v>
@@ -15262,7 +15262,7 @@
         <v>13.67</v>
       </c>
       <c r="M296" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N296" s="3">
         <v>51.94</v>
@@ -15276,7 +15276,7 @@
     </row>
     <row r="297" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B297" s="3">
         <v>16</v>
@@ -15312,7 +15312,7 @@
         <v>14.99</v>
       </c>
       <c r="M297" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N297" s="3">
         <v>55.67</v>
@@ -15326,7 +15326,7 @@
     </row>
     <row r="298" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B298" s="3">
         <v>17</v>
@@ -15359,7 +15359,7 @@
         <v>0.82</v>
       </c>
       <c r="M298" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N298" s="3">
         <v>6.75</v>
@@ -15373,7 +15373,7 @@
     </row>
     <row r="299" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B299" s="3">
         <v>18</v>
@@ -15409,7 +15409,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="M299" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N299" s="3">
         <v>17.079999999999998</v>
@@ -15423,7 +15423,7 @@
     </row>
     <row r="300" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B300" s="3">
         <v>19</v>
@@ -15459,7 +15459,7 @@
         <v>1.67</v>
       </c>
       <c r="M300" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N300" s="3">
         <v>11.78</v>
@@ -15473,7 +15473,7 @@
     </row>
     <row r="301" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B301" s="3">
         <v>20</v>
@@ -15509,7 +15509,7 @@
         <v>2.38</v>
       </c>
       <c r="M301" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N301" s="3">
         <v>14.48</v>
@@ -15523,7 +15523,7 @@
     </row>
     <row r="302" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B302" s="3">
         <v>21</v>
@@ -15559,7 +15559,7 @@
         <v>3.1</v>
       </c>
       <c r="M302" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N302" s="3">
         <v>17.22</v>
@@ -15573,7 +15573,7 @@
     </row>
     <row r="303" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B303" s="3">
         <v>22</v>
@@ -15609,7 +15609,7 @@
         <v>3.82</v>
       </c>
       <c r="M303" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N303" s="3">
         <v>19.940000000000001</v>
@@ -15623,7 +15623,7 @@
     </row>
     <row r="304" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B304" s="3">
         <v>23</v>
@@ -15659,7 +15659,7 @@
         <v>4.54</v>
       </c>
       <c r="M304" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N304" s="3">
         <v>22.669999999999998</v>
@@ -15673,7 +15673,7 @@
     </row>
     <row r="305" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B305" s="3">
         <v>24</v>
@@ -15709,7 +15709,7 @@
         <v>5.26</v>
       </c>
       <c r="M305" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N305" s="3">
         <v>25.39</v>
@@ -15723,7 +15723,7 @@
     </row>
     <row r="306" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A306" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B306" s="3">
         <v>25</v>
@@ -15759,7 +15759,7 @@
         <v>5.98</v>
       </c>
       <c r="M306" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N306" s="3">
         <v>28.11</v>
@@ -15773,7 +15773,7 @@
     </row>
     <row r="307" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B307" s="3">
         <v>26</v>
@@ -15809,7 +15809,7 @@
         <v>6.7</v>
       </c>
       <c r="M307" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N307" s="3">
         <v>30.839999999999996</v>
@@ -15823,7 +15823,7 @@
     </row>
     <row r="308" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A308" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B308" s="3">
         <v>27</v>
@@ -15859,7 +15859,7 @@
         <v>7.56</v>
       </c>
       <c r="M308" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N308" s="3">
         <v>33.809999999999995</v>
@@ -15873,7 +15873,7 @@
     </row>
     <row r="309" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B309" s="3">
         <v>28</v>
@@ -15909,7 +15909,7 @@
         <v>8.7799999999999994</v>
       </c>
       <c r="M309" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N309" s="3">
         <v>37.440000000000005</v>
@@ -15923,7 +15923,7 @@
     </row>
     <row r="310" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A310" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B310" s="3">
         <v>29</v>
@@ -15959,7 +15959,7 @@
         <v>10</v>
       </c>
       <c r="M310" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N310" s="3">
         <v>41.05</v>
@@ -15973,7 +15973,7 @@
     </row>
     <row r="311" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B311" s="3">
         <v>30</v>
@@ -16009,7 +16009,7 @@
         <v>11.22</v>
       </c>
       <c r="M311" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N311" s="3">
         <v>44.689999999999991</v>

</xml_diff>

<commit_message>
Update data with pine and elm fix
</commit_message>
<xml_diff>
--- a/data/trees-cost-benefit.xlsx
+++ b/data/trees-cost-benefit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunaynaagarwal/Documents/GitHub/capstone project/urbanforest_CBA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8B79CF-4294-E345-A996-1588281A320F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7416C0-E355-5E4D-990D-B3E0FFCBEBB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="460" windowWidth="25040" windowHeight="14100" xr2:uid="{2A928EC9-B78E-A343-8FB2-6539B0E6B4D7}"/>
   </bookViews>
@@ -59,13 +59,7 @@
     <t>blue palo verde</t>
   </si>
   <si>
-    <t xml:space="preserve">aleppo pine </t>
-  </si>
-  <si>
     <t>palo brea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chinese elm </t>
   </si>
   <si>
     <t>ben_property_value</t>
@@ -102,6 +96,12 @@
   </si>
   <si>
     <t>convenient</t>
+  </si>
+  <si>
+    <t>chinese elm</t>
+  </si>
+  <si>
+    <t>aleppo pine</t>
   </si>
 </sst>
 </file>
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C43A03F-FC37-6C4A-BA3B-39FF00DA712F}">
   <dimension ref="A1:S311"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A285" workbookViewId="0">
-      <selection activeCell="L311" sqref="L311"/>
+    <sheetView tabSelected="1" topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="A251" sqref="A251:A311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,34 +497,34 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -568,7 +568,7 @@
         <v>0.37</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N2" s="3">
         <v>8.5299999999999994</v>
@@ -618,7 +618,7 @@
         <v>0.47</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N3" s="3">
         <v>10.940000000000001</v>
@@ -668,7 +668,7 @@
         <v>0.63</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N4" s="3">
         <v>13.060000000000002</v>
@@ -718,7 +718,7 @@
         <v>1.03</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N5" s="3">
         <v>14.22</v>
@@ -768,7 +768,7 @@
         <v>1.42</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N6" s="3">
         <v>15.679999999999998</v>
@@ -818,7 +818,7 @@
         <v>1.81</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N7" s="3">
         <v>16.970000000000002</v>
@@ -868,7 +868,7 @@
         <v>2.21</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N8" s="3">
         <v>18.279999999999998</v>
@@ -918,7 +918,7 @@
         <v>2.6</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N9" s="3">
         <v>19.55</v>
@@ -968,7 +968,7 @@
         <v>2.99</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N10" s="3">
         <v>20.86</v>
@@ -1018,7 +1018,7 @@
         <v>3.39</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N11" s="3">
         <v>22.15</v>
@@ -1068,7 +1068,7 @@
         <v>3.78</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N12" s="3">
         <v>23.43</v>
@@ -1118,7 +1118,7 @@
         <v>4.18</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N13" s="3">
         <v>24.73</v>
@@ -1168,7 +1168,7 @@
         <v>4.57</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N14" s="3">
         <v>26.020000000000003</v>
@@ -1218,7 +1218,7 @@
         <v>5.04</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N15" s="3">
         <v>27.43</v>
@@ -1268,7 +1268,7 @@
         <v>5.6</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N16" s="3">
         <v>28.97</v>
@@ -1318,7 +1318,7 @@
         <v>6.15</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N17" s="3">
         <v>30.490000000000002</v>
@@ -1368,7 +1368,7 @@
         <v>6.71</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N18" s="3">
         <v>32.03</v>
@@ -1418,7 +1418,7 @@
         <v>7.26</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N19" s="3">
         <v>33.549999999999997</v>
@@ -1468,7 +1468,7 @@
         <v>7.8</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N20" s="3">
         <v>35.03</v>
@@ -1518,7 +1518,7 @@
         <v>8.31</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N21" s="3">
         <v>36.449999999999996</v>
@@ -1568,7 +1568,7 @@
         <v>8.81</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N22" s="3">
         <v>37.82</v>
@@ -1618,7 +1618,7 @@
         <v>9.2899999999999991</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N23" s="3">
         <v>39.14</v>
@@ -1668,7 +1668,7 @@
         <v>9.7200000000000006</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N24" s="3">
         <v>40.32</v>
@@ -1718,7 +1718,7 @@
         <v>10.14</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N25" s="3">
         <v>41.480000000000004</v>
@@ -1768,7 +1768,7 @@
         <v>10.53</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N26" s="3">
         <v>42.570000000000007</v>
@@ -1818,7 +1818,7 @@
         <v>10.93</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N27" s="3">
         <v>43.67</v>
@@ -1868,7 +1868,7 @@
         <v>11.31</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N28" s="3">
         <v>44.71</v>
@@ -1918,7 +1918,7 @@
         <v>11.66</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N29" s="3">
         <v>45.69</v>
@@ -1968,7 +1968,7 @@
         <v>12</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N30" s="3">
         <v>46.620000000000005</v>
@@ -2018,7 +2018,7 @@
         <v>12.34</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N31" s="3">
         <v>47.56</v>
@@ -2068,7 +2068,7 @@
         <v>12.68</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N32" s="3">
         <v>48.49</v>
@@ -2118,7 +2118,7 @@
         <v>0.37</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N33" s="3">
         <v>8.5299999999999994</v>
@@ -2168,7 +2168,7 @@
         <v>0.47</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N34" s="3">
         <v>10.940000000000001</v>
@@ -2218,7 +2218,7 @@
         <v>0.63</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N35" s="3">
         <v>13.060000000000002</v>
@@ -2268,7 +2268,7 @@
         <v>1.03</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N36" s="3">
         <v>14.22</v>
@@ -2318,7 +2318,7 @@
         <v>1.42</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N37" s="3">
         <v>15.679999999999998</v>
@@ -2368,7 +2368,7 @@
         <v>1.81</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N38" s="3">
         <v>16.970000000000002</v>
@@ -2418,7 +2418,7 @@
         <v>2.21</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N39" s="3">
         <v>18.279999999999998</v>
@@ -2468,7 +2468,7 @@
         <v>2.6</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N40" s="3">
         <v>19.55</v>
@@ -2518,7 +2518,7 @@
         <v>2.99</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N41" s="3">
         <v>20.86</v>
@@ -2568,7 +2568,7 @@
         <v>3.39</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N42" s="3">
         <v>22.15</v>
@@ -2618,7 +2618,7 @@
         <v>3.78</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N43" s="3">
         <v>23.43</v>
@@ -2668,7 +2668,7 @@
         <v>4.18</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N44" s="3">
         <v>24.73</v>
@@ -2718,7 +2718,7 @@
         <v>4.57</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N45" s="3">
         <v>26.020000000000003</v>
@@ -2768,7 +2768,7 @@
         <v>5.04</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N46" s="3">
         <v>27.43</v>
@@ -2818,7 +2818,7 @@
         <v>5.6</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N47" s="3">
         <v>28.97</v>
@@ -2868,7 +2868,7 @@
         <v>6.15</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N48" s="3">
         <v>30.490000000000002</v>
@@ -2918,7 +2918,7 @@
         <v>6.71</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N49" s="3">
         <v>32.03</v>
@@ -2968,7 +2968,7 @@
         <v>0.37</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N50" s="3">
         <v>8.5299999999999994</v>
@@ -3018,7 +3018,7 @@
         <v>0.47</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N51" s="3">
         <v>10.940000000000001</v>
@@ -3068,7 +3068,7 @@
         <v>0.63</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N52" s="3">
         <v>13.060000000000002</v>
@@ -3118,7 +3118,7 @@
         <v>1.03</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N53" s="3">
         <v>14.22</v>
@@ -3168,7 +3168,7 @@
         <v>1.42</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N54" s="3">
         <v>15.679999999999998</v>
@@ -3218,7 +3218,7 @@
         <v>1.81</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N55" s="3">
         <v>16.970000000000002</v>
@@ -3268,7 +3268,7 @@
         <v>2.21</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N56" s="3">
         <v>18.279999999999998</v>
@@ -3318,7 +3318,7 @@
         <v>2.6</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N57" s="3">
         <v>19.55</v>
@@ -3368,7 +3368,7 @@
         <v>2.99</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N58" s="3">
         <v>20.86</v>
@@ -3418,7 +3418,7 @@
         <v>3.39</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N59" s="3">
         <v>22.15</v>
@@ -3468,7 +3468,7 @@
         <v>3.78</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N60" s="3">
         <v>23.43</v>
@@ -3518,7 +3518,7 @@
         <v>4.18</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N61" s="3">
         <v>24.73</v>
@@ -3568,7 +3568,7 @@
         <v>4.57</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N62" s="3">
         <v>26.020000000000003</v>
@@ -3618,7 +3618,7 @@
         <v>5.04</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N63" s="3">
         <v>27.43</v>
@@ -3668,7 +3668,7 @@
         <v>0.37</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N64" s="3">
         <v>4.3599999999999994</v>
@@ -3718,7 +3718,7 @@
         <v>0.5</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N65" s="3">
         <v>5.93</v>
@@ -3768,7 +3768,7 @@
         <v>0.9</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N66" s="3">
         <v>7.620000000000001</v>
@@ -3818,7 +3818,7 @@
         <v>1.48</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N67" s="3">
         <v>9.3199999999999985</v>
@@ -3868,7 +3868,7 @@
         <v>2.06</v>
       </c>
       <c r="M68" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N68" s="3">
         <v>11.060000000000002</v>
@@ -3918,7 +3918,7 @@
         <v>2.64</v>
       </c>
       <c r="M69" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N69" s="3">
         <v>12.780000000000001</v>
@@ -3968,7 +3968,7 @@
         <v>3.21</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N70" s="3">
         <v>14.52</v>
@@ -4018,7 +4018,7 @@
         <v>3.79</v>
       </c>
       <c r="M71" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N71" s="3">
         <v>16.240000000000002</v>
@@ -4068,7 +4068,7 @@
         <v>4.37</v>
       </c>
       <c r="M72" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N72" s="3">
         <v>17.97</v>
@@ -4118,7 +4118,7 @@
         <v>4.95</v>
       </c>
       <c r="M73" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N73" s="3">
         <v>19.7</v>
@@ -4168,7 +4168,7 @@
         <v>5.55</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N74" s="3">
         <v>21.51</v>
@@ -4218,7 +4218,7 @@
         <v>6.29</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N75" s="3">
         <v>23.729999999999997</v>
@@ -4268,7 +4268,7 @@
         <v>6.97</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N76" s="3">
         <v>25.77</v>
@@ -4318,7 +4318,7 @@
         <v>7.59</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N77" s="3">
         <v>27.62</v>
@@ -4368,7 +4368,7 @@
         <v>8.16</v>
       </c>
       <c r="M78" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N78" s="3">
         <v>29.319999999999997</v>
@@ -4418,7 +4418,7 @@
         <v>8.82</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N79" s="3">
         <v>31.310000000000002</v>
@@ -4468,7 +4468,7 @@
         <v>9.34</v>
       </c>
       <c r="M80" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N80" s="3">
         <v>32.879999999999995</v>
@@ -4518,7 +4518,7 @@
         <v>9.7899999999999991</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N81" s="3">
         <v>34.119999999999997</v>
@@ -4568,7 +4568,7 @@
         <v>10.19</v>
       </c>
       <c r="M82" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N82" s="3">
         <v>35.44</v>
@@ -4618,7 +4618,7 @@
         <v>10.57</v>
       </c>
       <c r="M83" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N83" s="3">
         <v>36.570000000000007</v>
@@ -4668,7 +4668,7 @@
         <v>10.93</v>
       </c>
       <c r="M84" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N84" s="3">
         <v>37.650000000000006</v>
@@ -4718,7 +4718,7 @@
         <v>11.26</v>
       </c>
       <c r="M85" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N85" s="3">
         <v>38.639999999999993</v>
@@ -4768,7 +4768,7 @@
         <v>11.57</v>
       </c>
       <c r="M86" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N86" s="3">
         <v>39.57</v>
@@ -4818,7 +4818,7 @@
         <v>11.85</v>
       </c>
       <c r="M87" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N87" s="3">
         <v>40.410000000000004</v>
@@ -4868,7 +4868,7 @@
         <v>12.11</v>
       </c>
       <c r="M88" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N88" s="3">
         <v>41.18</v>
@@ -4918,7 +4918,7 @@
         <v>12.35</v>
       </c>
       <c r="M89" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N89" s="3">
         <v>41.9</v>
@@ -4968,7 +4968,7 @@
         <v>12.56</v>
       </c>
       <c r="M90" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N90" s="3">
         <v>42.54</v>
@@ -5018,7 +5018,7 @@
         <v>12.78</v>
       </c>
       <c r="M91" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N91" s="3">
         <v>43.18</v>
@@ -5068,7 +5068,7 @@
         <v>12.97</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N92" s="3">
         <v>43.75</v>
@@ -5118,7 +5118,7 @@
         <v>13.16</v>
       </c>
       <c r="M93" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N93" s="3">
         <v>44.319999999999993</v>
@@ -5168,7 +5168,7 @@
         <v>13.32</v>
       </c>
       <c r="M94" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N94" s="3">
         <v>44.81</v>
@@ -5218,7 +5218,7 @@
         <v>0.37</v>
       </c>
       <c r="M95" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N95" s="3">
         <v>4.3599999999999994</v>
@@ -5268,7 +5268,7 @@
         <v>0.5</v>
       </c>
       <c r="M96" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N96" s="3">
         <v>5.93</v>
@@ -5318,7 +5318,7 @@
         <v>0.9</v>
       </c>
       <c r="M97" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N97" s="3">
         <v>7.620000000000001</v>
@@ -5368,7 +5368,7 @@
         <v>1.48</v>
       </c>
       <c r="M98" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N98" s="3">
         <v>9.3199999999999985</v>
@@ -5418,7 +5418,7 @@
         <v>2.06</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N99" s="3">
         <v>11.060000000000002</v>
@@ -5468,7 +5468,7 @@
         <v>2.64</v>
       </c>
       <c r="M100" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N100" s="3">
         <v>12.780000000000001</v>
@@ -5518,7 +5518,7 @@
         <v>3.21</v>
       </c>
       <c r="M101" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N101" s="3">
         <v>14.52</v>
@@ -5568,7 +5568,7 @@
         <v>3.79</v>
       </c>
       <c r="M102" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N102" s="3">
         <v>16.240000000000002</v>
@@ -5618,7 +5618,7 @@
         <v>4.37</v>
       </c>
       <c r="M103" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N103" s="3">
         <v>17.97</v>
@@ -5668,7 +5668,7 @@
         <v>4.95</v>
       </c>
       <c r="M104" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N104" s="3">
         <v>19.7</v>
@@ -5718,7 +5718,7 @@
         <v>5.55</v>
       </c>
       <c r="M105" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N105" s="3">
         <v>21.51</v>
@@ -5768,7 +5768,7 @@
         <v>6.29</v>
       </c>
       <c r="M106" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N106" s="3">
         <v>23.729999999999997</v>
@@ -5818,7 +5818,7 @@
         <v>6.97</v>
       </c>
       <c r="M107" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N107" s="3">
         <v>25.77</v>
@@ -5868,7 +5868,7 @@
         <v>7.59</v>
       </c>
       <c r="M108" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N108" s="3">
         <v>27.62</v>
@@ -5918,7 +5918,7 @@
         <v>8.16</v>
       </c>
       <c r="M109" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N109" s="3">
         <v>29.319999999999997</v>
@@ -5968,7 +5968,7 @@
         <v>0.37</v>
       </c>
       <c r="M110" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N110" s="3">
         <v>4.3599999999999994</v>
@@ -6018,7 +6018,7 @@
         <v>0.5</v>
       </c>
       <c r="M111" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N111" s="3">
         <v>5.93</v>
@@ -6068,7 +6068,7 @@
         <v>0.9</v>
       </c>
       <c r="M112" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N112" s="3">
         <v>7.620000000000001</v>
@@ -6118,7 +6118,7 @@
         <v>1.48</v>
       </c>
       <c r="M113" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N113" s="3">
         <v>9.3199999999999985</v>
@@ -6168,7 +6168,7 @@
         <v>2.06</v>
       </c>
       <c r="M114" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N114" s="3">
         <v>11.060000000000002</v>
@@ -6218,7 +6218,7 @@
         <v>2.64</v>
       </c>
       <c r="M115" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N115" s="3">
         <v>12.780000000000001</v>
@@ -6268,7 +6268,7 @@
         <v>3.21</v>
       </c>
       <c r="M116" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N116" s="3">
         <v>14.52</v>
@@ -6318,7 +6318,7 @@
         <v>3.79</v>
       </c>
       <c r="M117" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N117" s="3">
         <v>16.240000000000002</v>
@@ -6368,7 +6368,7 @@
         <v>4.37</v>
       </c>
       <c r="M118" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N118" s="3">
         <v>17.97</v>
@@ -6418,7 +6418,7 @@
         <v>4.95</v>
       </c>
       <c r="M119" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N119" s="3">
         <v>19.7</v>
@@ -6468,7 +6468,7 @@
         <v>5.55</v>
       </c>
       <c r="M120" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N120" s="3">
         <v>21.51</v>
@@ -6518,7 +6518,7 @@
         <v>6.29</v>
       </c>
       <c r="M121" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N121" s="3">
         <v>23.729999999999997</v>
@@ -6568,7 +6568,7 @@
         <v>6.97</v>
       </c>
       <c r="M122" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N122" s="3">
         <v>25.77</v>
@@ -6618,7 +6618,7 @@
         <v>7.59</v>
       </c>
       <c r="M123" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N123" s="3">
         <v>27.62</v>
@@ -6668,7 +6668,7 @@
         <v>8.16</v>
       </c>
       <c r="M124" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N124" s="3">
         <v>29.319999999999997</v>
@@ -6718,7 +6718,7 @@
         <v>13.32</v>
       </c>
       <c r="M125" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N125" s="3">
         <v>31</v>
@@ -6732,7 +6732,7 @@
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B126" s="3">
         <v>0</v>
@@ -6768,7 +6768,7 @@
         <v>0.3</v>
       </c>
       <c r="M126" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N126" s="3">
         <v>5.45</v>
@@ -6782,7 +6782,7 @@
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B127" s="3">
         <v>1</v>
@@ -6818,7 +6818,7 @@
         <v>0.4</v>
       </c>
       <c r="M127" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N127" s="3">
         <v>6.9700000000000006</v>
@@ -6832,7 +6832,7 @@
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B128" s="3">
         <v>2</v>
@@ -6868,7 +6868,7 @@
         <v>0.49</v>
       </c>
       <c r="M128" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N128" s="3">
         <v>8.3899999999999988</v>
@@ -6882,7 +6882,7 @@
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B129" s="3">
         <v>3</v>
@@ -6918,7 +6918,7 @@
         <v>0.63</v>
       </c>
       <c r="M129" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N129" s="3">
         <v>9.4300000000000015</v>
@@ -6932,7 +6932,7 @@
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B130" s="3">
         <v>4</v>
@@ -6968,7 +6968,7 @@
         <v>0.77</v>
       </c>
       <c r="M130" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N130" s="3">
         <v>10.51</v>
@@ -6982,7 +6982,7 @@
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B131" s="3">
         <v>5</v>
@@ -7018,7 +7018,7 @@
         <v>0.9</v>
       </c>
       <c r="M131" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N131" s="3">
         <v>11.51</v>
@@ -7032,7 +7032,7 @@
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B132" s="3">
         <v>6</v>
@@ -7068,7 +7068,7 @@
         <v>1.04</v>
       </c>
       <c r="M132" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N132" s="3">
         <v>12.509999999999998</v>
@@ -7082,7 +7082,7 @@
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B133" s="3">
         <v>7</v>
@@ -7118,7 +7118,7 @@
         <v>1.17</v>
       </c>
       <c r="M133" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N133" s="3">
         <v>13.54</v>
@@ -7132,7 +7132,7 @@
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B134" s="3">
         <v>8</v>
@@ -7168,7 +7168,7 @@
         <v>1.31</v>
       </c>
       <c r="M134" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N134" s="3">
         <v>14.58</v>
@@ -7182,7 +7182,7 @@
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B135" s="3">
         <v>9</v>
@@ -7218,7 +7218,7 @@
         <v>1.45</v>
       </c>
       <c r="M135" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N135" s="3">
         <v>15.62</v>
@@ -7232,7 +7232,7 @@
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B136" s="3">
         <v>10</v>
@@ -7268,7 +7268,7 @@
         <v>1.58</v>
       </c>
       <c r="M136" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N136" s="3">
         <v>16.649999999999999</v>
@@ -7282,7 +7282,7 @@
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B137" s="3">
         <v>11</v>
@@ -7318,7 +7318,7 @@
         <v>1.72</v>
       </c>
       <c r="M137" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N137" s="3">
         <v>17.689999999999998</v>
@@ -7332,7 +7332,7 @@
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B138" s="3">
         <v>12</v>
@@ -7368,7 +7368,7 @@
         <v>1.85</v>
       </c>
       <c r="M138" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N138" s="3">
         <v>18.720000000000002</v>
@@ -7382,7 +7382,7 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B139" s="3">
         <v>13</v>
@@ -7418,7 +7418,7 @@
         <v>2.06</v>
       </c>
       <c r="M139" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N139" s="3">
         <v>19.86</v>
@@ -7432,7 +7432,7 @@
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B140" s="3">
         <v>14</v>
@@ -7468,7 +7468,7 @@
         <v>2.33</v>
       </c>
       <c r="M140" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N140" s="3">
         <v>21.11</v>
@@ -7482,7 +7482,7 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B141" s="3">
         <v>15</v>
@@ -7518,7 +7518,7 @@
         <v>2.6</v>
       </c>
       <c r="M141" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N141" s="3">
         <v>22.350000000000005</v>
@@ -7532,7 +7532,7 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B142" s="3">
         <v>16</v>
@@ -7568,7 +7568,7 @@
         <v>2.87</v>
       </c>
       <c r="M142" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N142" s="3">
         <v>23.610000000000003</v>
@@ -7582,7 +7582,7 @@
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B143" s="3">
         <v>17</v>
@@ -7618,7 +7618,7 @@
         <v>3.14</v>
       </c>
       <c r="M143" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N143" s="3">
         <v>24.840000000000003</v>
@@ -7632,7 +7632,7 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B144" s="3">
         <v>18</v>
@@ -7668,7 +7668,7 @@
         <v>3.41</v>
       </c>
       <c r="M144" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N144" s="3">
         <v>26.08</v>
@@ -7682,7 +7682,7 @@
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B145" s="3">
         <v>19</v>
@@ -7718,7 +7718,7 @@
         <v>3.69</v>
       </c>
       <c r="M145" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N145" s="3">
         <v>27.36</v>
@@ -7732,7 +7732,7 @@
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B146" s="3">
         <v>20</v>
@@ -7768,7 +7768,7 @@
         <v>3.96</v>
       </c>
       <c r="M146" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N146" s="3">
         <v>28.59</v>
@@ -7782,7 +7782,7 @@
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B147" s="3">
         <v>21</v>
@@ -7818,7 +7818,7 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="M147" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N147" s="3">
         <v>29.84</v>
@@ -7832,7 +7832,7 @@
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B148" s="3">
         <v>22</v>
@@ -7868,7 +7868,7 @@
         <v>4.5</v>
       </c>
       <c r="M148" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N148" s="3">
         <v>31.090000000000003</v>
@@ -7882,7 +7882,7 @@
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B149" s="3">
         <v>23</v>
@@ -7918,7 +7918,7 @@
         <v>4.7699999999999996</v>
       </c>
       <c r="M149" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N149" s="3">
         <v>32.339999999999996</v>
@@ -7932,7 +7932,7 @@
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B150" s="3">
         <v>24</v>
@@ -7968,7 +7968,7 @@
         <v>5.04</v>
       </c>
       <c r="M150" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N150" s="3">
         <v>33.57</v>
@@ -7982,7 +7982,7 @@
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B151" s="3">
         <v>25</v>
@@ -8018,7 +8018,7 @@
         <v>5.31</v>
       </c>
       <c r="M151" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N151" s="3">
         <v>34.830000000000005</v>
@@ -8032,7 +8032,7 @@
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B152" s="3">
         <v>26</v>
@@ -8068,7 +8068,7 @@
         <v>5.59</v>
       </c>
       <c r="M152" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N152" s="3">
         <v>36.099999999999994</v>
@@ -8082,7 +8082,7 @@
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B153" s="3">
         <v>27</v>
@@ -8118,7 +8118,7 @@
         <v>5.86</v>
       </c>
       <c r="M153" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N153" s="3">
         <v>37.32</v>
@@ -8132,7 +8132,7 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B154" s="3">
         <v>28</v>
@@ -8168,7 +8168,7 @@
         <v>6.13</v>
       </c>
       <c r="M154" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N154" s="3">
         <v>38.590000000000011</v>
@@ -8182,7 +8182,7 @@
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B155" s="3">
         <v>29</v>
@@ -8218,7 +8218,7 @@
         <v>6.48</v>
       </c>
       <c r="M155" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N155" s="3">
         <v>39.870000000000005</v>
@@ -8232,7 +8232,7 @@
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B156" s="3">
         <v>30</v>
@@ -8268,7 +8268,7 @@
         <v>6.93</v>
       </c>
       <c r="M156" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N156" s="3">
         <v>41.209999999999994</v>
@@ -8282,7 +8282,7 @@
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B157" s="3">
         <v>0</v>
@@ -8318,7 +8318,7 @@
         <v>0.3</v>
       </c>
       <c r="M157" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N157" s="3">
         <v>5.45</v>
@@ -8332,7 +8332,7 @@
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B158" s="3">
         <v>1</v>
@@ -8368,7 +8368,7 @@
         <v>0.4</v>
       </c>
       <c r="M158" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N158" s="3">
         <v>6.9700000000000006</v>
@@ -8382,7 +8382,7 @@
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B159" s="3">
         <v>2</v>
@@ -8418,7 +8418,7 @@
         <v>0.49</v>
       </c>
       <c r="M159" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N159" s="3">
         <v>8.3899999999999988</v>
@@ -8432,7 +8432,7 @@
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B160" s="3">
         <v>3</v>
@@ -8468,7 +8468,7 @@
         <v>0.63</v>
       </c>
       <c r="M160" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N160" s="3">
         <v>9.4300000000000015</v>
@@ -8482,7 +8482,7 @@
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B161" s="3">
         <v>4</v>
@@ -8518,7 +8518,7 @@
         <v>0.77</v>
       </c>
       <c r="M161" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N161" s="3">
         <v>10.51</v>
@@ -8532,7 +8532,7 @@
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B162" s="3">
         <v>5</v>
@@ -8568,7 +8568,7 @@
         <v>0.9</v>
       </c>
       <c r="M162" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N162" s="3">
         <v>11.51</v>
@@ -8582,7 +8582,7 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B163" s="3">
         <v>6</v>
@@ -8618,7 +8618,7 @@
         <v>1.04</v>
       </c>
       <c r="M163" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N163" s="3">
         <v>12.509999999999998</v>
@@ -8632,7 +8632,7 @@
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B164" s="3">
         <v>7</v>
@@ -8668,7 +8668,7 @@
         <v>1.17</v>
       </c>
       <c r="M164" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N164" s="3">
         <v>13.54</v>
@@ -8682,7 +8682,7 @@
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B165" s="3">
         <v>8</v>
@@ -8718,7 +8718,7 @@
         <v>1.31</v>
       </c>
       <c r="M165" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N165" s="3">
         <v>14.58</v>
@@ -8732,7 +8732,7 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B166" s="3">
         <v>9</v>
@@ -8768,7 +8768,7 @@
         <v>1.45</v>
       </c>
       <c r="M166" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N166" s="3">
         <v>15.62</v>
@@ -8782,7 +8782,7 @@
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B167" s="3">
         <v>10</v>
@@ -8818,7 +8818,7 @@
         <v>1.58</v>
       </c>
       <c r="M167" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N167" s="3">
         <v>16.649999999999999</v>
@@ -8832,7 +8832,7 @@
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B168" s="3">
         <v>11</v>
@@ -8868,7 +8868,7 @@
         <v>1.72</v>
       </c>
       <c r="M168" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N168" s="3">
         <v>17.689999999999998</v>
@@ -8882,7 +8882,7 @@
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B169" s="3">
         <v>12</v>
@@ -8918,7 +8918,7 @@
         <v>1.85</v>
       </c>
       <c r="M169" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N169" s="3">
         <v>18.720000000000002</v>
@@ -8932,7 +8932,7 @@
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B170" s="3">
         <v>13</v>
@@ -8968,7 +8968,7 @@
         <v>2.06</v>
       </c>
       <c r="M170" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N170" s="3">
         <v>19.86</v>
@@ -8982,7 +8982,7 @@
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B171" s="3">
         <v>14</v>
@@ -9018,7 +9018,7 @@
         <v>2.33</v>
       </c>
       <c r="M171" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N171" s="3">
         <v>21.11</v>
@@ -9032,7 +9032,7 @@
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B172" s="3">
         <v>15</v>
@@ -9068,7 +9068,7 @@
         <v>2.6</v>
       </c>
       <c r="M172" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N172" s="3">
         <v>22.350000000000005</v>
@@ -9082,7 +9082,7 @@
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B173" s="3">
         <v>16</v>
@@ -9118,7 +9118,7 @@
         <v>0.3</v>
       </c>
       <c r="M173" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N173" s="3">
         <v>5.45</v>
@@ -9132,7 +9132,7 @@
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B174" s="3">
         <v>17</v>
@@ -9168,7 +9168,7 @@
         <v>0.4</v>
       </c>
       <c r="M174" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N174" s="3">
         <v>6.9700000000000006</v>
@@ -9182,7 +9182,7 @@
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B175" s="3">
         <v>18</v>
@@ -9218,7 +9218,7 @@
         <v>0.49</v>
       </c>
       <c r="M175" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N175" s="3">
         <v>8.3899999999999988</v>
@@ -9232,7 +9232,7 @@
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B176" s="3">
         <v>19</v>
@@ -9268,7 +9268,7 @@
         <v>0.63</v>
       </c>
       <c r="M176" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N176" s="3">
         <v>9.4300000000000015</v>
@@ -9282,7 +9282,7 @@
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B177" s="3">
         <v>20</v>
@@ -9318,7 +9318,7 @@
         <v>0.77</v>
       </c>
       <c r="M177" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N177" s="3">
         <v>10.51</v>
@@ -9332,7 +9332,7 @@
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B178" s="3">
         <v>21</v>
@@ -9368,7 +9368,7 @@
         <v>0.9</v>
       </c>
       <c r="M178" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N178" s="3">
         <v>11.51</v>
@@ -9382,7 +9382,7 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B179" s="3">
         <v>22</v>
@@ -9418,7 +9418,7 @@
         <v>1.04</v>
       </c>
       <c r="M179" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N179" s="3">
         <v>12.509999999999998</v>
@@ -9432,7 +9432,7 @@
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B180" s="3">
         <v>23</v>
@@ -9468,7 +9468,7 @@
         <v>1.17</v>
       </c>
       <c r="M180" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N180" s="3">
         <v>13.54</v>
@@ -9482,7 +9482,7 @@
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B181" s="3">
         <v>24</v>
@@ -9518,7 +9518,7 @@
         <v>1.31</v>
       </c>
       <c r="M181" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N181" s="3">
         <v>14.58</v>
@@ -9532,7 +9532,7 @@
     </row>
     <row r="182" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B182" s="3">
         <v>25</v>
@@ -9568,7 +9568,7 @@
         <v>1.45</v>
       </c>
       <c r="M182" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N182" s="3">
         <v>15.62</v>
@@ -9582,7 +9582,7 @@
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B183" s="3">
         <v>26</v>
@@ -9618,7 +9618,7 @@
         <v>1.58</v>
       </c>
       <c r="M183" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N183" s="3">
         <v>16.649999999999999</v>
@@ -9632,7 +9632,7 @@
     </row>
     <row r="184" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B184" s="3">
         <v>27</v>
@@ -9668,7 +9668,7 @@
         <v>1.72</v>
       </c>
       <c r="M184" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N184" s="3">
         <v>17.689999999999998</v>
@@ -9682,7 +9682,7 @@
     </row>
     <row r="185" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B185" s="3">
         <v>28</v>
@@ -9718,7 +9718,7 @@
         <v>1.85</v>
       </c>
       <c r="M185" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N185" s="3">
         <v>18.720000000000002</v>
@@ -9732,7 +9732,7 @@
     </row>
     <row r="186" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B186" s="3">
         <v>29</v>
@@ -9768,7 +9768,7 @@
         <v>2.06</v>
       </c>
       <c r="M186" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N186" s="3">
         <v>19.86</v>
@@ -9782,7 +9782,7 @@
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B187" s="3">
         <v>30</v>
@@ -9818,7 +9818,7 @@
         <v>2.33</v>
       </c>
       <c r="M187" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N187" s="3">
         <v>21.11</v>
@@ -9832,7 +9832,7 @@
     </row>
     <row r="188" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B188" s="3">
         <v>0</v>
@@ -9868,7 +9868,7 @@
         <v>0.51</v>
       </c>
       <c r="M188" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N188" s="3">
         <v>6.28</v>
@@ -9882,7 +9882,7 @@
     </row>
     <row r="189" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B189" s="3">
         <v>1</v>
@@ -9918,7 +9918,7 @@
         <v>0.6</v>
       </c>
       <c r="M189" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N189" s="3">
         <v>7.4599999999999991</v>
@@ -9932,7 +9932,7 @@
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B190" s="3">
         <v>2</v>
@@ -9968,7 +9968,7 @@
         <v>0.7</v>
       </c>
       <c r="M190" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N190" s="3">
         <v>9.1000000000000014</v>
@@ -9982,7 +9982,7 @@
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B191" s="3">
         <v>3</v>
@@ -10018,7 +10018,7 @@
         <v>0.81</v>
       </c>
       <c r="M191" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N191" s="3">
         <v>9.5400000000000009</v>
@@ -10032,7 +10032,7 @@
     </row>
     <row r="192" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B192" s="3">
         <v>4</v>
@@ -10068,7 +10068,7 @@
         <v>0.96</v>
       </c>
       <c r="M192" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N192" s="3">
         <v>9.870000000000001</v>
@@ -10082,7 +10082,7 @@
     </row>
     <row r="193" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B193" s="3">
         <v>5</v>
@@ -10118,7 +10118,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="M193" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N193" s="3">
         <v>10.199999999999999</v>
@@ -10132,7 +10132,7 @@
     </row>
     <row r="194" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B194" s="3">
         <v>6</v>
@@ -10168,7 +10168,7 @@
         <v>1.22</v>
       </c>
       <c r="M194" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N194" s="3">
         <v>10.5</v>
@@ -10182,7 +10182,7 @@
     </row>
     <row r="195" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B195" s="3">
         <v>7</v>
@@ -10218,7 +10218,7 @@
         <v>1.34</v>
       </c>
       <c r="M195" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N195" s="3">
         <v>10.79</v>
@@ -10232,7 +10232,7 @@
     </row>
     <row r="196" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B196" s="3">
         <v>8</v>
@@ -10268,7 +10268,7 @@
         <v>1.44</v>
       </c>
       <c r="M196" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N196" s="3">
         <v>11.04</v>
@@ -10282,7 +10282,7 @@
     </row>
     <row r="197" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B197" s="3">
         <v>9</v>
@@ -10318,7 +10318,7 @@
         <v>1.54</v>
       </c>
       <c r="M197" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N197" s="3">
         <v>11.280000000000001</v>
@@ -10332,7 +10332,7 @@
     </row>
     <row r="198" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B198" s="3">
         <v>10</v>
@@ -10368,7 +10368,7 @@
         <v>1.65</v>
       </c>
       <c r="M198" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N198" s="3">
         <v>11.49</v>
@@ -10382,7 +10382,7 @@
     </row>
     <row r="199" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B199" s="3">
         <v>11</v>
@@ -10418,7 +10418,7 @@
         <v>1.72</v>
       </c>
       <c r="M199" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N199" s="3">
         <v>11.68</v>
@@ -10432,7 +10432,7 @@
     </row>
     <row r="200" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B200" s="3">
         <v>12</v>
@@ -10468,7 +10468,7 @@
         <v>1.79</v>
       </c>
       <c r="M200" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N200" s="3">
         <v>11.86</v>
@@ -10482,7 +10482,7 @@
     </row>
     <row r="201" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B201" s="3">
         <v>13</v>
@@ -10518,7 +10518,7 @@
         <v>1.86</v>
       </c>
       <c r="M201" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N201" s="3">
         <v>12.009999999999998</v>
@@ -10532,7 +10532,7 @@
     </row>
     <row r="202" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B202" s="3">
         <v>14</v>
@@ -10568,7 +10568,7 @@
         <v>1.92</v>
       </c>
       <c r="M202" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N202" s="3">
         <v>12.17</v>
@@ -10582,7 +10582,7 @@
     </row>
     <row r="203" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B203" s="3">
         <v>15</v>
@@ -10618,7 +10618,7 @@
         <v>1.98</v>
       </c>
       <c r="M203" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N203" s="3">
         <v>12.31</v>
@@ -10632,7 +10632,7 @@
     </row>
     <row r="204" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B204" s="3">
         <v>16</v>
@@ -10668,7 +10668,7 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="M204" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N204" s="3">
         <v>12.430000000000001</v>
@@ -10682,7 +10682,7 @@
     </row>
     <row r="205" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B205" s="3">
         <v>17</v>
@@ -10718,7 +10718,7 @@
         <v>2.08</v>
       </c>
       <c r="M205" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N205" s="3">
         <v>12.55</v>
@@ -10732,7 +10732,7 @@
     </row>
     <row r="206" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B206" s="3">
         <v>18</v>
@@ -10768,7 +10768,7 @@
         <v>2.13</v>
       </c>
       <c r="M206" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N206" s="3">
         <v>12.669999999999998</v>
@@ -10782,7 +10782,7 @@
     </row>
     <row r="207" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B207" s="3">
         <v>19</v>
@@ -10818,7 +10818,7 @@
         <v>2.17</v>
       </c>
       <c r="M207" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N207" s="3">
         <v>12.76</v>
@@ -10832,7 +10832,7 @@
     </row>
     <row r="208" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B208" s="3">
         <v>20</v>
@@ -10868,7 +10868,7 @@
         <v>2.21</v>
       </c>
       <c r="M208" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N208" s="3">
         <v>12.86</v>
@@ -10882,7 +10882,7 @@
     </row>
     <row r="209" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B209" s="3">
         <v>21</v>
@@ -10918,7 +10918,7 @@
         <v>2.25</v>
       </c>
       <c r="M209" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N209" s="3">
         <v>12.96</v>
@@ -10932,7 +10932,7 @@
     </row>
     <row r="210" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B210" s="3">
         <v>22</v>
@@ -10968,7 +10968,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="M210" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N210" s="3">
         <v>13.030000000000001</v>
@@ -10982,7 +10982,7 @@
     </row>
     <row r="211" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B211" s="3">
         <v>23</v>
@@ -11018,7 +11018,7 @@
         <v>2.31</v>
       </c>
       <c r="M211" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N211" s="3">
         <v>13.090000000000002</v>
@@ -11032,7 +11032,7 @@
     </row>
     <row r="212" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B212" s="3">
         <v>24</v>
@@ -11068,7 +11068,7 @@
         <v>2.34</v>
       </c>
       <c r="M212" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N212" s="3">
         <v>13.16</v>
@@ -11082,7 +11082,7 @@
     </row>
     <row r="213" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B213" s="3">
         <v>25</v>
@@ -11118,7 +11118,7 @@
         <v>2.37</v>
       </c>
       <c r="M213" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N213" s="3">
         <v>13.239999999999998</v>
@@ -11132,7 +11132,7 @@
     </row>
     <row r="214" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B214" s="3">
         <v>26</v>
@@ -11168,7 +11168,7 @@
         <v>2.4</v>
       </c>
       <c r="M214" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N214" s="3">
         <v>13.309999999999999</v>
@@ -11182,7 +11182,7 @@
     </row>
     <row r="215" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B215" s="3">
         <v>27</v>
@@ -11218,7 +11218,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="M215" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N215" s="3">
         <v>13.379999999999999</v>
@@ -11232,7 +11232,7 @@
     </row>
     <row r="216" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B216" s="3">
         <v>28</v>
@@ -11268,7 +11268,7 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="M216" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N216" s="3">
         <v>13.419999999999998</v>
@@ -11282,7 +11282,7 @@
     </row>
     <row r="217" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B217" s="3">
         <v>29</v>
@@ -11318,7 +11318,7 @@
         <v>2.4700000000000002</v>
       </c>
       <c r="M217" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N217" s="3">
         <v>13.48</v>
@@ -11332,7 +11332,7 @@
     </row>
     <row r="218" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B218" s="3">
         <v>30</v>
@@ -11368,7 +11368,7 @@
         <v>2.5</v>
       </c>
       <c r="M218" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N218" s="3">
         <v>13.54</v>
@@ -11382,7 +11382,7 @@
     </row>
     <row r="219" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B219" s="3">
         <v>0</v>
@@ -11418,7 +11418,7 @@
         <v>0.51</v>
       </c>
       <c r="M219" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N219" s="3">
         <v>6.28</v>
@@ -11432,7 +11432,7 @@
     </row>
     <row r="220" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B220" s="3">
         <v>1</v>
@@ -11468,7 +11468,7 @@
         <v>0.6</v>
       </c>
       <c r="M220" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N220" s="3">
         <v>7.4599999999999991</v>
@@ -11482,7 +11482,7 @@
     </row>
     <row r="221" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B221" s="3">
         <v>2</v>
@@ -11518,7 +11518,7 @@
         <v>0.7</v>
       </c>
       <c r="M221" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N221" s="3">
         <v>9.1000000000000014</v>
@@ -11532,7 +11532,7 @@
     </row>
     <row r="222" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B222" s="3">
         <v>3</v>
@@ -11568,7 +11568,7 @@
         <v>0.81</v>
       </c>
       <c r="M222" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N222" s="3">
         <v>9.5400000000000009</v>
@@ -11582,7 +11582,7 @@
     </row>
     <row r="223" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B223" s="3">
         <v>4</v>
@@ -11618,7 +11618,7 @@
         <v>0.96</v>
       </c>
       <c r="M223" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N223" s="3">
         <v>9.870000000000001</v>
@@ -11632,7 +11632,7 @@
     </row>
     <row r="224" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B224" s="3">
         <v>5</v>
@@ -11668,7 +11668,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="M224" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N224" s="3">
         <v>10.199999999999999</v>
@@ -11682,7 +11682,7 @@
     </row>
     <row r="225" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B225" s="3">
         <v>6</v>
@@ -11718,7 +11718,7 @@
         <v>1.22</v>
       </c>
       <c r="M225" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N225" s="3">
         <v>10.5</v>
@@ -11732,7 +11732,7 @@
     </row>
     <row r="226" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B226" s="3">
         <v>7</v>
@@ -11768,7 +11768,7 @@
         <v>1.34</v>
       </c>
       <c r="M226" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N226" s="3">
         <v>10.79</v>
@@ -11782,7 +11782,7 @@
     </row>
     <row r="227" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B227" s="3">
         <v>8</v>
@@ -11818,7 +11818,7 @@
         <v>1.44</v>
       </c>
       <c r="M227" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N227" s="3">
         <v>11.04</v>
@@ -11832,7 +11832,7 @@
     </row>
     <row r="228" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B228" s="3">
         <v>9</v>
@@ -11868,7 +11868,7 @@
         <v>1.54</v>
       </c>
       <c r="M228" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N228" s="3">
         <v>11.280000000000001</v>
@@ -11882,7 +11882,7 @@
     </row>
     <row r="229" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B229" s="3">
         <v>10</v>
@@ -11918,7 +11918,7 @@
         <v>1.65</v>
       </c>
       <c r="M229" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N229" s="3">
         <v>11.49</v>
@@ -11932,7 +11932,7 @@
     </row>
     <row r="230" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B230" s="3">
         <v>11</v>
@@ -11968,7 +11968,7 @@
         <v>1.72</v>
       </c>
       <c r="M230" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N230" s="3">
         <v>11.68</v>
@@ -11982,7 +11982,7 @@
     </row>
     <row r="231" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B231" s="3">
         <v>12</v>
@@ -12018,7 +12018,7 @@
         <v>1.79</v>
       </c>
       <c r="M231" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N231" s="3">
         <v>11.86</v>
@@ -12032,7 +12032,7 @@
     </row>
     <row r="232" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B232" s="3">
         <v>13</v>
@@ -12068,7 +12068,7 @@
         <v>1.86</v>
       </c>
       <c r="M232" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N232" s="3">
         <v>12.009999999999998</v>
@@ -12082,7 +12082,7 @@
     </row>
     <row r="233" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B233" s="3">
         <v>14</v>
@@ -12118,7 +12118,7 @@
         <v>1.92</v>
       </c>
       <c r="M233" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N233" s="3">
         <v>12.17</v>
@@ -12132,7 +12132,7 @@
     </row>
     <row r="234" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B234" s="3">
         <v>15</v>
@@ -12168,7 +12168,7 @@
         <v>1.98</v>
       </c>
       <c r="M234" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N234" s="3">
         <v>12.31</v>
@@ -12182,7 +12182,7 @@
     </row>
     <row r="235" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B235" s="3">
         <v>16</v>
@@ -12218,7 +12218,7 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="M235" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N235" s="3">
         <v>12.430000000000001</v>
@@ -12232,7 +12232,7 @@
     </row>
     <row r="236" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B236" s="3">
         <v>17</v>
@@ -12268,7 +12268,7 @@
         <v>2.08</v>
       </c>
       <c r="M236" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N236" s="3">
         <v>6.28</v>
@@ -12282,7 +12282,7 @@
     </row>
     <row r="237" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B237" s="3">
         <v>18</v>
@@ -12318,7 +12318,7 @@
         <v>0.6</v>
       </c>
       <c r="M237" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N237" s="3">
         <v>7.4599999999999991</v>
@@ -12332,7 +12332,7 @@
     </row>
     <row r="238" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B238" s="3">
         <v>19</v>
@@ -12368,7 +12368,7 @@
         <v>0.7</v>
       </c>
       <c r="M238" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N238" s="3">
         <v>9.1000000000000014</v>
@@ -12382,7 +12382,7 @@
     </row>
     <row r="239" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B239" s="3">
         <v>20</v>
@@ -12418,7 +12418,7 @@
         <v>0.81</v>
       </c>
       <c r="M239" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N239" s="3">
         <v>9.5400000000000009</v>
@@ -12432,7 +12432,7 @@
     </row>
     <row r="240" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B240" s="3">
         <v>21</v>
@@ -12468,7 +12468,7 @@
         <v>0.96</v>
       </c>
       <c r="M240" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N240" s="3">
         <v>9.870000000000001</v>
@@ -12482,7 +12482,7 @@
     </row>
     <row r="241" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B241" s="3">
         <v>22</v>
@@ -12518,7 +12518,7 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="M241" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N241" s="3">
         <v>10.199999999999999</v>
@@ -12532,7 +12532,7 @@
     </row>
     <row r="242" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B242" s="3">
         <v>23</v>
@@ -12568,7 +12568,7 @@
         <v>1.22</v>
       </c>
       <c r="M242" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N242" s="3">
         <v>10.5</v>
@@ -12582,7 +12582,7 @@
     </row>
     <row r="243" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B243" s="3">
         <v>24</v>
@@ -12618,7 +12618,7 @@
         <v>1.34</v>
       </c>
       <c r="M243" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N243" s="3">
         <v>10.79</v>
@@ -12632,7 +12632,7 @@
     </row>
     <row r="244" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B244" s="3">
         <v>25</v>
@@ -12668,7 +12668,7 @@
         <v>1.44</v>
       </c>
       <c r="M244" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N244" s="3">
         <v>11.04</v>
@@ -12682,7 +12682,7 @@
     </row>
     <row r="245" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B245" s="3">
         <v>26</v>
@@ -12718,7 +12718,7 @@
         <v>1.54</v>
       </c>
       <c r="M245" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N245" s="3">
         <v>11.280000000000001</v>
@@ -12732,7 +12732,7 @@
     </row>
     <row r="246" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B246" s="3">
         <v>27</v>
@@ -12768,7 +12768,7 @@
         <v>1.65</v>
       </c>
       <c r="M246" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N246" s="3">
         <v>11.49</v>
@@ -12782,7 +12782,7 @@
     </row>
     <row r="247" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B247" s="3">
         <v>28</v>
@@ -12818,7 +12818,7 @@
         <v>1.72</v>
       </c>
       <c r="M247" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N247" s="3">
         <v>11.68</v>
@@ -12832,7 +12832,7 @@
     </row>
     <row r="248" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B248" s="3">
         <v>29</v>
@@ -12868,7 +12868,7 @@
         <v>1.79</v>
       </c>
       <c r="M248" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N248" s="3">
         <v>11.86</v>
@@ -12882,7 +12882,7 @@
     </row>
     <row r="249" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B249" s="3">
         <v>30</v>
@@ -12918,7 +12918,7 @@
         <v>1.86</v>
       </c>
       <c r="M249" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N249" s="3">
         <v>12.009999999999998</v>
@@ -12932,7 +12932,7 @@
     </row>
     <row r="250" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B250" s="3">
         <v>0</v>
@@ -12965,7 +12965,7 @@
         <v>0.82</v>
       </c>
       <c r="M250" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N250" s="3">
         <v>6.75</v>
@@ -12979,7 +12979,7 @@
     </row>
     <row r="251" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B251" s="3">
         <v>1</v>
@@ -13015,7 +13015,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="M251" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N251" s="3">
         <v>17.079999999999998</v>
@@ -13029,7 +13029,7 @@
     </row>
     <row r="252" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B252" s="3">
         <v>2</v>
@@ -13065,7 +13065,7 @@
         <v>1.67</v>
       </c>
       <c r="M252" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N252" s="3">
         <v>11.78</v>
@@ -13079,7 +13079,7 @@
     </row>
     <row r="253" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B253" s="3">
         <v>3</v>
@@ -13115,7 +13115,7 @@
         <v>2.38</v>
       </c>
       <c r="M253" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N253" s="3">
         <v>14.48</v>
@@ -13129,7 +13129,7 @@
     </row>
     <row r="254" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B254" s="3">
         <v>4</v>
@@ -13165,7 +13165,7 @@
         <v>3.1</v>
       </c>
       <c r="M254" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N254" s="3">
         <v>17.22</v>
@@ -13179,7 +13179,7 @@
     </row>
     <row r="255" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B255" s="3">
         <v>5</v>
@@ -13215,7 +13215,7 @@
         <v>3.82</v>
       </c>
       <c r="M255" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N255" s="3">
         <v>19.940000000000001</v>
@@ -13229,7 +13229,7 @@
     </row>
     <row r="256" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B256" s="3">
         <v>6</v>
@@ -13265,7 +13265,7 @@
         <v>4.54</v>
       </c>
       <c r="M256" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N256" s="3">
         <v>22.669999999999998</v>
@@ -13279,7 +13279,7 @@
     </row>
     <row r="257" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B257" s="3">
         <v>7</v>
@@ -13315,7 +13315,7 @@
         <v>5.26</v>
       </c>
       <c r="M257" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N257" s="3">
         <v>25.39</v>
@@ -13329,7 +13329,7 @@
     </row>
     <row r="258" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B258" s="3">
         <v>8</v>
@@ -13365,7 +13365,7 @@
         <v>5.98</v>
       </c>
       <c r="M258" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N258" s="3">
         <v>28.11</v>
@@ -13379,7 +13379,7 @@
     </row>
     <row r="259" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B259" s="3">
         <v>9</v>
@@ -13415,7 +13415,7 @@
         <v>6.7</v>
       </c>
       <c r="M259" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N259" s="3">
         <v>30.839999999999996</v>
@@ -13429,7 +13429,7 @@
     </row>
     <row r="260" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B260" s="3">
         <v>10</v>
@@ -13465,7 +13465,7 @@
         <v>7.56</v>
       </c>
       <c r="M260" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N260" s="3">
         <v>33.809999999999995</v>
@@ -13479,7 +13479,7 @@
     </row>
     <row r="261" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B261" s="3">
         <v>11</v>
@@ -13515,7 +13515,7 @@
         <v>8.7799999999999994</v>
       </c>
       <c r="M261" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N261" s="3">
         <v>37.440000000000005</v>
@@ -13529,7 +13529,7 @@
     </row>
     <row r="262" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B262" s="3">
         <v>12</v>
@@ -13565,7 +13565,7 @@
         <v>10</v>
       </c>
       <c r="M262" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N262" s="3">
         <v>41.05</v>
@@ -13579,7 +13579,7 @@
     </row>
     <row r="263" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B263" s="3">
         <v>13</v>
@@ -13615,7 +13615,7 @@
         <v>11.22</v>
       </c>
       <c r="M263" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N263" s="3">
         <v>44.689999999999991</v>
@@ -13629,7 +13629,7 @@
     </row>
     <row r="264" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B264" s="3">
         <v>14</v>
@@ -13665,7 +13665,7 @@
         <v>12.45</v>
       </c>
       <c r="M264" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N264" s="3">
         <v>48.319999999999993</v>
@@ -13679,7 +13679,7 @@
     </row>
     <row r="265" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B265" s="3">
         <v>15</v>
@@ -13715,7 +13715,7 @@
         <v>13.67</v>
       </c>
       <c r="M265" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N265" s="3">
         <v>51.94</v>
@@ -13729,7 +13729,7 @@
     </row>
     <row r="266" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B266" s="3">
         <v>16</v>
@@ -13765,7 +13765,7 @@
         <v>14.99</v>
       </c>
       <c r="M266" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N266" s="3">
         <v>55.67</v>
@@ -13779,7 +13779,7 @@
     </row>
     <row r="267" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B267" s="3">
         <v>17</v>
@@ -13815,7 +13815,7 @@
         <v>16.11</v>
       </c>
       <c r="M267" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N267" s="3">
         <v>59.180000000000007</v>
@@ -13829,7 +13829,7 @@
     </row>
     <row r="268" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B268" s="3">
         <v>18</v>
@@ -13865,7 +13865,7 @@
         <v>17.329999999999998</v>
       </c>
       <c r="M268" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N268" s="3">
         <v>62.809999999999995</v>
@@ -13879,7 +13879,7 @@
     </row>
     <row r="269" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B269" s="3">
         <v>19</v>
@@ -13915,7 +13915,7 @@
         <v>18.55</v>
       </c>
       <c r="M269" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N269" s="3">
         <v>66.45</v>
@@ -13929,7 +13929,7 @@
     </row>
     <row r="270" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B270" s="3">
         <v>20</v>
@@ -13965,7 +13965,7 @@
         <v>19.77</v>
       </c>
       <c r="M270" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N270" s="3">
         <v>70.05</v>
@@ -13979,7 +13979,7 @@
     </row>
     <row r="271" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B271" s="3">
         <v>21</v>
@@ -14015,7 +14015,7 @@
         <v>21</v>
       </c>
       <c r="M271" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N271" s="3">
         <v>73.69</v>
@@ -14029,7 +14029,7 @@
     </row>
     <row r="272" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B272" s="3">
         <v>22</v>
@@ -14065,7 +14065,7 @@
         <v>22.22</v>
       </c>
       <c r="M272" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N272" s="3">
         <v>77.319999999999993</v>
@@ -14079,7 +14079,7 @@
     </row>
     <row r="273" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B273" s="3">
         <v>23</v>
@@ -14115,7 +14115,7 @@
         <v>23.74</v>
       </c>
       <c r="M273" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N273" s="3">
         <v>81.56</v>
@@ -14129,7 +14129,7 @@
     </row>
     <row r="274" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B274" s="3">
         <v>24</v>
@@ -14165,7 +14165,7 @@
         <v>25.34</v>
       </c>
       <c r="M274" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N274" s="3">
         <v>85.95</v>
@@ -14179,7 +14179,7 @@
     </row>
     <row r="275" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B275" s="3">
         <v>25</v>
@@ -14215,7 +14215,7 @@
         <v>26.95</v>
       </c>
       <c r="M275" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N275" s="3">
         <v>90.36</v>
@@ -14229,7 +14229,7 @@
     </row>
     <row r="276" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B276" s="3">
         <v>26</v>
@@ -14265,7 +14265,7 @@
         <v>28.73</v>
       </c>
       <c r="M276" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N276" s="3">
         <v>95.259999999999991</v>
@@ -14279,7 +14279,7 @@
     </row>
     <row r="277" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B277" s="3">
         <v>27</v>
@@ -14315,7 +14315,7 @@
         <v>30.51</v>
       </c>
       <c r="M277" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N277" s="3">
         <v>100.15</v>
@@ -14329,7 +14329,7 @@
     </row>
     <row r="278" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B278" s="3">
         <v>28</v>
@@ -14365,7 +14365,7 @@
         <v>31.85</v>
       </c>
       <c r="M278" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N278" s="3">
         <v>103.83000000000001</v>
@@ -14379,7 +14379,7 @@
     </row>
     <row r="279" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B279" s="3">
         <v>29</v>
@@ -14415,7 +14415,7 @@
         <v>33.630000000000003</v>
       </c>
       <c r="M279" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N279" s="3">
         <v>108.73000000000002</v>
@@ -14429,7 +14429,7 @@
     </row>
     <row r="280" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B280" s="3">
         <v>30</v>
@@ -14465,7 +14465,7 @@
         <v>34.97</v>
       </c>
       <c r="M280" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N280" s="3">
         <v>112.4</v>
@@ -14479,7 +14479,7 @@
     </row>
     <row r="281" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B281" s="3">
         <v>0</v>
@@ -14512,7 +14512,7 @@
         <v>0.82</v>
       </c>
       <c r="M281" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N281" s="3">
         <v>6.75</v>
@@ -14526,7 +14526,7 @@
     </row>
     <row r="282" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B282" s="3">
         <v>1</v>
@@ -14562,7 +14562,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="M282" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N282" s="3">
         <v>17.079999999999998</v>
@@ -14576,7 +14576,7 @@
     </row>
     <row r="283" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B283" s="3">
         <v>2</v>
@@ -14612,7 +14612,7 @@
         <v>1.67</v>
       </c>
       <c r="M283" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N283" s="3">
         <v>11.78</v>
@@ -14626,7 +14626,7 @@
     </row>
     <row r="284" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B284" s="3">
         <v>3</v>
@@ -14662,7 +14662,7 @@
         <v>2.38</v>
       </c>
       <c r="M284" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N284" s="3">
         <v>14.48</v>
@@ -14676,7 +14676,7 @@
     </row>
     <row r="285" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B285" s="3">
         <v>4</v>
@@ -14712,7 +14712,7 @@
         <v>3.1</v>
       </c>
       <c r="M285" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N285" s="3">
         <v>17.22</v>
@@ -14726,7 +14726,7 @@
     </row>
     <row r="286" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B286" s="3">
         <v>5</v>
@@ -14762,7 +14762,7 @@
         <v>3.82</v>
       </c>
       <c r="M286" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N286" s="3">
         <v>19.940000000000001</v>
@@ -14776,7 +14776,7 @@
     </row>
     <row r="287" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B287" s="3">
         <v>6</v>
@@ -14812,7 +14812,7 @@
         <v>4.54</v>
       </c>
       <c r="M287" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N287" s="3">
         <v>22.669999999999998</v>
@@ -14826,7 +14826,7 @@
     </row>
     <row r="288" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B288" s="3">
         <v>7</v>
@@ -14862,7 +14862,7 @@
         <v>5.26</v>
       </c>
       <c r="M288" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N288" s="3">
         <v>25.39</v>
@@ -14876,7 +14876,7 @@
     </row>
     <row r="289" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B289" s="3">
         <v>8</v>
@@ -14912,7 +14912,7 @@
         <v>5.98</v>
       </c>
       <c r="M289" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N289" s="3">
         <v>28.11</v>
@@ -14926,7 +14926,7 @@
     </row>
     <row r="290" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B290" s="3">
         <v>9</v>
@@ -14962,7 +14962,7 @@
         <v>6.7</v>
       </c>
       <c r="M290" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N290" s="3">
         <v>30.839999999999996</v>
@@ -14976,7 +14976,7 @@
     </row>
     <row r="291" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B291" s="3">
         <v>10</v>
@@ -15012,7 +15012,7 @@
         <v>7.56</v>
       </c>
       <c r="M291" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N291" s="3">
         <v>33.809999999999995</v>
@@ -15026,7 +15026,7 @@
     </row>
     <row r="292" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B292" s="3">
         <v>11</v>
@@ -15062,7 +15062,7 @@
         <v>8.7799999999999994</v>
       </c>
       <c r="M292" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N292" s="3">
         <v>37.440000000000005</v>
@@ -15076,7 +15076,7 @@
     </row>
     <row r="293" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B293" s="3">
         <v>12</v>
@@ -15112,7 +15112,7 @@
         <v>10</v>
       </c>
       <c r="M293" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N293" s="3">
         <v>41.05</v>
@@ -15126,7 +15126,7 @@
     </row>
     <row r="294" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B294" s="3">
         <v>13</v>
@@ -15162,7 +15162,7 @@
         <v>11.22</v>
       </c>
       <c r="M294" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N294" s="3">
         <v>44.689999999999991</v>
@@ -15176,7 +15176,7 @@
     </row>
     <row r="295" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B295" s="3">
         <v>14</v>
@@ -15212,7 +15212,7 @@
         <v>12.45</v>
       </c>
       <c r="M295" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N295" s="3">
         <v>48.319999999999993</v>
@@ -15226,7 +15226,7 @@
     </row>
     <row r="296" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B296" s="3">
         <v>15</v>
@@ -15262,7 +15262,7 @@
         <v>13.67</v>
       </c>
       <c r="M296" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N296" s="3">
         <v>51.94</v>
@@ -15276,7 +15276,7 @@
     </row>
     <row r="297" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B297" s="3">
         <v>16</v>
@@ -15312,7 +15312,7 @@
         <v>14.99</v>
       </c>
       <c r="M297" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N297" s="3">
         <v>55.67</v>
@@ -15326,7 +15326,7 @@
     </row>
     <row r="298" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B298" s="3">
         <v>17</v>
@@ -15359,7 +15359,7 @@
         <v>0.82</v>
       </c>
       <c r="M298" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N298" s="3">
         <v>6.75</v>
@@ -15373,7 +15373,7 @@
     </row>
     <row r="299" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B299" s="3">
         <v>18</v>
@@ -15409,7 +15409,7 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="M299" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N299" s="3">
         <v>17.079999999999998</v>
@@ -15423,7 +15423,7 @@
     </row>
     <row r="300" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B300" s="3">
         <v>19</v>
@@ -15459,7 +15459,7 @@
         <v>1.67</v>
       </c>
       <c r="M300" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N300" s="3">
         <v>11.78</v>
@@ -15473,7 +15473,7 @@
     </row>
     <row r="301" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B301" s="3">
         <v>20</v>
@@ -15509,7 +15509,7 @@
         <v>2.38</v>
       </c>
       <c r="M301" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N301" s="3">
         <v>14.48</v>
@@ -15523,7 +15523,7 @@
     </row>
     <row r="302" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A302" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B302" s="3">
         <v>21</v>
@@ -15559,7 +15559,7 @@
         <v>3.1</v>
       </c>
       <c r="M302" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N302" s="3">
         <v>17.22</v>
@@ -15573,7 +15573,7 @@
     </row>
     <row r="303" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B303" s="3">
         <v>22</v>
@@ -15609,7 +15609,7 @@
         <v>3.82</v>
       </c>
       <c r="M303" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N303" s="3">
         <v>19.940000000000001</v>
@@ -15623,7 +15623,7 @@
     </row>
     <row r="304" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A304" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B304" s="3">
         <v>23</v>
@@ -15659,7 +15659,7 @@
         <v>4.54</v>
       </c>
       <c r="M304" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N304" s="3">
         <v>22.669999999999998</v>
@@ -15673,7 +15673,7 @@
     </row>
     <row r="305" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A305" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B305" s="3">
         <v>24</v>
@@ -15709,7 +15709,7 @@
         <v>5.26</v>
       </c>
       <c r="M305" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N305" s="3">
         <v>25.39</v>
@@ -15723,7 +15723,7 @@
     </row>
     <row r="306" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A306" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B306" s="3">
         <v>25</v>
@@ -15759,7 +15759,7 @@
         <v>5.98</v>
       </c>
       <c r="M306" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N306" s="3">
         <v>28.11</v>
@@ -15773,7 +15773,7 @@
     </row>
     <row r="307" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A307" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B307" s="3">
         <v>26</v>
@@ -15809,7 +15809,7 @@
         <v>6.7</v>
       </c>
       <c r="M307" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N307" s="3">
         <v>30.839999999999996</v>
@@ -15823,7 +15823,7 @@
     </row>
     <row r="308" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A308" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B308" s="3">
         <v>27</v>
@@ -15859,7 +15859,7 @@
         <v>7.56</v>
       </c>
       <c r="M308" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N308" s="3">
         <v>33.809999999999995</v>
@@ -15873,7 +15873,7 @@
     </row>
     <row r="309" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A309" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B309" s="3">
         <v>28</v>
@@ -15909,7 +15909,7 @@
         <v>8.7799999999999994</v>
       </c>
       <c r="M309" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N309" s="3">
         <v>37.440000000000005</v>
@@ -15923,7 +15923,7 @@
     </row>
     <row r="310" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A310" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B310" s="3">
         <v>29</v>
@@ -15959,7 +15959,7 @@
         <v>10</v>
       </c>
       <c r="M310" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N310" s="3">
         <v>41.05</v>
@@ -15973,7 +15973,7 @@
     </row>
     <row r="311" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A311" s="3" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B311" s="3">
         <v>30</v>
@@ -16009,7 +16009,7 @@
         <v>11.22</v>
       </c>
       <c r="M311" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N311" s="3">
         <v>44.689999999999991</v>

</xml_diff>